<commit_message>
Fixed initialization of storage systems
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -6538,7 +6538,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="3">
@@ -6549,7 +6549,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="4">
@@ -6560,7 +6560,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="5">
@@ -6571,7 +6571,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="6">
@@ -6582,7 +6582,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="7">
@@ -6593,7 +6593,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="8">
@@ -6604,7 +6604,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="9">
@@ -6615,7 +6615,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="10">
@@ -6626,7 +6626,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="11">
@@ -6637,7 +6637,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="12">
@@ -6648,7 +6648,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="13">
@@ -6659,7 +6659,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="14">
@@ -6670,7 +6670,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="15">
@@ -6681,7 +6681,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="16">
@@ -6692,7 +6692,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="17">
@@ -6703,7 +6703,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="18">
@@ -6714,7 +6714,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="19">
@@ -6725,7 +6725,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="20">
@@ -6736,7 +6736,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="21">
@@ -6747,7 +6747,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="22">
@@ -6758,7 +6758,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="23">
@@ -6769,7 +6769,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="24">
@@ -6780,7 +6780,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="25">
@@ -6791,7 +6791,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="26">
@@ -6802,7 +6802,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="27">
@@ -6813,7 +6813,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="28">
@@ -6824,7 +6824,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="29">
@@ -6835,7 +6835,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="30">
@@ -6846,7 +6846,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="31">
@@ -6857,7 +6857,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="32">
@@ -6868,7 +6868,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="33">
@@ -6879,7 +6879,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="34">
@@ -6890,7 +6890,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="35">
@@ -6901,7 +6901,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="36">
@@ -6912,7 +6912,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="37">
@@ -6923,7 +6923,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="38">
@@ -6934,7 +6934,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="39">
@@ -6945,7 +6945,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="40">
@@ -6956,7 +6956,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="41">
@@ -6967,7 +6967,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="42">
@@ -6978,7 +6978,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="43">
@@ -6989,7 +6989,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="44">
@@ -7000,7 +7000,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="45">
@@ -7011,7 +7011,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="46">
@@ -7022,7 +7022,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="47">
@@ -7033,7 +7033,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="48">
@@ -7044,7 +7044,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="49">
@@ -7055,7 +7055,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="50">
@@ -7066,7 +7066,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="51">
@@ -7077,7 +7077,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="52">
@@ -7088,7 +7088,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="53">
@@ -7099,7 +7099,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="54">
@@ -7110,7 +7110,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="55">
@@ -7121,7 +7121,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="56">
@@ -7132,7 +7132,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="57">
@@ -7143,7 +7143,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="58">
@@ -7154,7 +7154,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="59">
@@ -7165,7 +7165,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="60">
@@ -7176,7 +7176,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="61">
@@ -7187,7 +7187,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="62">
@@ -7198,7 +7198,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="63">
@@ -7209,7 +7209,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="64">
@@ -7220,7 +7220,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="65">
@@ -7231,7 +7231,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="66">
@@ -7242,7 +7242,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="67">
@@ -7253,7 +7253,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="68">
@@ -7264,7 +7264,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="69">
@@ -7275,7 +7275,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="70">
@@ -7286,7 +7286,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="71">
@@ -7297,7 +7297,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="72">
@@ -7308,7 +7308,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="73">
@@ -7319,7 +7319,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="74">
@@ -7330,7 +7330,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="75">
@@ -7341,7 +7341,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="76">
@@ -7352,7 +7352,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="77">
@@ -7363,7 +7363,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="78">
@@ -7374,7 +7374,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="79">
@@ -7385,7 +7385,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="80">
@@ -7396,7 +7396,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="81">
@@ -7407,7 +7407,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="82">
@@ -7418,7 +7418,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="83">
@@ -7429,7 +7429,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="84">
@@ -7440,7 +7440,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="85">
@@ -7451,7 +7451,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="86">
@@ -7462,7 +7462,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="87">
@@ -7473,7 +7473,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="88">
@@ -7484,7 +7484,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="89">
@@ -7495,7 +7495,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="90">
@@ -7506,7 +7506,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="91">
@@ -7517,7 +7517,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="92">
@@ -7528,7 +7528,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="93">
@@ -7539,7 +7539,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="94">
@@ -7550,7 +7550,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with multi-dry year transfer limits and contingency conservation volume
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -490,7 +490,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>4742768.410980233</v>
+        <v>14046425.72236278</v>
       </c>
     </row>
     <row r="5">
@@ -545,7 +545,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>4859427.462889392</v>
+        <v>13885032.54876038</v>
       </c>
     </row>
     <row r="10">
@@ -567,7 +567,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>4505660.803390387</v>
+        <v>14374259.44341646</v>
       </c>
     </row>
     <row r="12">
@@ -578,7 +578,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>5637227.325860668</v>
+        <v>13930227.32586067</v>
       </c>
     </row>
     <row r="13">
@@ -600,7 +600,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>5290941.306954685</v>
+        <v>13583941.30695468</v>
       </c>
     </row>
     <row r="15">
@@ -1073,7 +1073,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3778080.380690524</v>
+        <v>15380436.54137731</v>
       </c>
     </row>
     <row r="58">
@@ -1227,7 +1227,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>4505660.803390387</v>
+        <v>14374259.44341646</v>
       </c>
     </row>
     <row r="72">
@@ -1238,7 +1238,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>5592642.040205687</v>
+        <v>13885642.04020569</v>
       </c>
     </row>
     <row r="73">
@@ -1480,7 +1480,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>4562134.043308323</v>
+        <v>14296162.12402704</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1549,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>501.2898235000002</v>
       </c>
     </row>
     <row r="5">
@@ -1604,7 +1604,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>363.3748749999996</v>
       </c>
     </row>
     <row r="10">
@@ -1626,7 +1626,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>781.5028450000001</v>
       </c>
     </row>
     <row r="12">
@@ -2132,7 +2132,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1641.453089</v>
       </c>
     </row>
     <row r="58">
@@ -2286,7 +2286,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>781.5028450000001</v>
       </c>
     </row>
     <row r="72">
@@ -2539,7 +2539,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>714.7553419999996</v>
       </c>
     </row>
   </sheetData>
@@ -10021,7 +10021,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1178.593372</v>
       </c>
     </row>
     <row r="5">
@@ -10076,7 +10076,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1040.674875</v>
       </c>
     </row>
     <row r="10">
@@ -10098,7 +10098,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1458.802845</v>
       </c>
     </row>
     <row r="12">
@@ -10109,7 +10109,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>121.404176</v>
       </c>
     </row>
     <row r="13">
@@ -10131,7 +10131,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>530.6550559999996</v>
       </c>
     </row>
     <row r="15">
@@ -10604,7 +10604,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>2318.753089</v>
       </c>
     </row>
     <row r="58">
@@ -10758,7 +10758,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1458.802845</v>
       </c>
     </row>
     <row r="72">
@@ -10769,7 +10769,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>174.0654459999996</v>
       </c>
     </row>
     <row r="73">
@@ -11011,7 +11011,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1392.055342</v>
       </c>
     </row>
   </sheetData>
@@ -11080,7 +11080,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>677.3035485</v>
       </c>
     </row>
     <row r="5">
@@ -11135,7 +11135,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>677.3000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -11157,7 +11157,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>677.3000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -11168,7 +11168,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>121.404176</v>
       </c>
     </row>
     <row r="13">
@@ -11190,7 +11190,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>530.6550559999996</v>
       </c>
     </row>
     <row r="15">
@@ -11663,7 +11663,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>677.3000000000001</v>
       </c>
     </row>
     <row r="58">
@@ -11817,7 +11817,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>677.3000000000001</v>
       </c>
     </row>
     <row r="72">
@@ -11828,7 +11828,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>174.0654459999996</v>
       </c>
     </row>
     <row r="73">
@@ -12070,7 +12070,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>677.3000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more results for export
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>14046425.72236278</v>
+        <v>74609684.54060502</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +501,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +534,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="9">
@@ -545,7 +545,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>13885032.54876038</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="10">
@@ -556,7 +556,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="11">
@@ -567,7 +567,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>14374259.44341646</v>
+        <v>34761233.58251005</v>
       </c>
     </row>
     <row r="12">
@@ -578,7 +578,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>13930227.32586067</v>
+        <v>34877823.78496338</v>
       </c>
     </row>
     <row r="13">
@@ -589,7 +589,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>5739944.084542823</v>
+        <v>35328480.30778956</v>
       </c>
     </row>
     <row r="14">
@@ -600,7 +600,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>13583941.30695468</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="15">
@@ -611,7 +611,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="16">
@@ -622,7 +622,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="17">
@@ -633,7 +633,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="18">
@@ -644,7 +644,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="19">
@@ -655,7 +655,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="20">
@@ -666,7 +666,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="22">
@@ -688,7 +688,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="23">
@@ -699,7 +699,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="24">
@@ -710,7 +710,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="25">
@@ -721,7 +721,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="27">
@@ -743,7 +743,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="28">
@@ -754,7 +754,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="29">
@@ -765,7 +765,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="30">
@@ -776,7 +776,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="31">
@@ -787,7 +787,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="32">
@@ -798,7 +798,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="33">
@@ -809,7 +809,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="34">
@@ -820,7 +820,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="35">
@@ -831,7 +831,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="36">
@@ -842,7 +842,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="37">
@@ -853,7 +853,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="38">
@@ -864,7 +864,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="39">
@@ -875,7 +875,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="40">
@@ -886,7 +886,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="41">
@@ -897,7 +897,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="42">
@@ -908,7 +908,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="43">
@@ -919,7 +919,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="45">
@@ -941,7 +941,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="46">
@@ -952,7 +952,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="48">
@@ -974,7 +974,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="49">
@@ -985,7 +985,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="50">
@@ -996,7 +996,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="51">
@@ -1007,7 +1007,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="52">
@@ -1018,7 +1018,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="53">
@@ -1029,7 +1029,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="54">
@@ -1040,7 +1040,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="55">
@@ -1051,7 +1051,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="56">
@@ -1062,7 +1062,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="57">
@@ -1073,7 +1073,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>15380436.54137731</v>
+        <v>34981027.87197478</v>
       </c>
     </row>
     <row r="58">
@@ -1084,7 +1084,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="59">
@@ -1095,7 +1095,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="60">
@@ -1106,7 +1106,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="61">
@@ -1117,7 +1117,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="62">
@@ -1128,7 +1128,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="63">
@@ -1139,7 +1139,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="64">
@@ -1150,7 +1150,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="65">
@@ -1161,7 +1161,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="66">
@@ -1172,7 +1172,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="67">
@@ -1183,7 +1183,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="68">
@@ -1194,7 +1194,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="69">
@@ -1205,7 +1205,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="70">
@@ -1216,7 +1216,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="71">
@@ -1227,7 +1227,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>14374259.44341646</v>
+        <v>34796027.60825985</v>
       </c>
     </row>
     <row r="72">
@@ -1238,7 +1238,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>13885642.04020569</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="73">
@@ -1249,7 +1249,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="74">
@@ -1260,7 +1260,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="75">
@@ -1271,7 +1271,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="76">
@@ -1282,7 +1282,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="77">
@@ -1293,7 +1293,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="78">
@@ -1304,7 +1304,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="79">
@@ -1315,7 +1315,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="80">
@@ -1326,7 +1326,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="81">
@@ -1337,7 +1337,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="82">
@@ -1348,7 +1348,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="83">
@@ -1359,7 +1359,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="84">
@@ -1370,7 +1370,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="85">
@@ -1381,7 +1381,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="86">
@@ -1392,7 +1392,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="87">
@@ -1403,7 +1403,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="88">
@@ -1414,7 +1414,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="89">
@@ -1425,7 +1425,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="90">
@@ -1436,7 +1436,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="91">
@@ -1447,7 +1447,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>5739944.084542823</v>
+        <v>34812722.64019499</v>
       </c>
     </row>
     <row r="92">
@@ -1458,7 +1458,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>5739944.084542823</v>
+        <v>34934793.77734198</v>
       </c>
     </row>
     <row r="93">
@@ -1469,7 +1469,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>5739914.06165315</v>
+        <v>34636862.16021674</v>
       </c>
     </row>
     <row r="94">
@@ -1480,7 +1480,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>14296162.12402704</v>
+        <v>34721480.65978038</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>501.2898235000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1604,7 +1604,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>363.3748749999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1626,7 +1626,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>781.5028450000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2132,7 +2132,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>1641.453089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2286,7 +2286,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>781.5028450000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2539,7 +2539,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>714.7553419999996</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="3">
@@ -4715,7 +4715,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="4">
@@ -4726,7 +4726,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="5">
@@ -4737,7 +4737,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="6">
@@ -4748,7 +4748,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="7">
@@ -4759,7 +4759,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="8">
@@ -4770,7 +4770,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="9">
@@ -4781,7 +4781,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="10">
@@ -4792,7 +4792,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="11">
@@ -4803,7 +4803,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="12">
@@ -4814,7 +4814,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="13">
@@ -4825,7 +4825,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="14">
@@ -4836,7 +4836,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="15">
@@ -4847,7 +4847,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="16">
@@ -4858,7 +4858,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="17">
@@ -4869,7 +4869,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="18">
@@ -4880,7 +4880,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="19">
@@ -4891,7 +4891,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="20">
@@ -4902,7 +4902,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="21">
@@ -4913,7 +4913,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="22">
@@ -4924,7 +4924,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="23">
@@ -4935,7 +4935,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="24">
@@ -4946,7 +4946,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="25">
@@ -4957,7 +4957,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="26">
@@ -4968,7 +4968,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="27">
@@ -4979,7 +4979,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="28">
@@ -4990,7 +4990,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="29">
@@ -5001,7 +5001,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="30">
@@ -5012,7 +5012,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="31">
@@ -5023,7 +5023,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="32">
@@ -5034,7 +5034,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="33">
@@ -5045,7 +5045,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="34">
@@ -5056,7 +5056,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="35">
@@ -5067,7 +5067,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="36">
@@ -5078,7 +5078,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="37">
@@ -5089,7 +5089,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="38">
@@ -5100,7 +5100,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="39">
@@ -5111,7 +5111,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="40">
@@ -5122,7 +5122,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="41">
@@ -5133,7 +5133,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="42">
@@ -5144,7 +5144,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="43">
@@ -5155,7 +5155,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="44">
@@ -5166,7 +5166,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="45">
@@ -5177,7 +5177,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="46">
@@ -5188,7 +5188,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="47">
@@ -5199,7 +5199,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="48">
@@ -5210,7 +5210,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="49">
@@ -5221,7 +5221,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="50">
@@ -5232,7 +5232,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="51">
@@ -5243,7 +5243,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="52">
@@ -5254,7 +5254,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="53">
@@ -5265,7 +5265,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="54">
@@ -5276,7 +5276,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="55">
@@ -5287,7 +5287,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="56">
@@ -5298,7 +5298,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="57">
@@ -5309,7 +5309,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="58">
@@ -5320,7 +5320,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="59">
@@ -5331,7 +5331,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="60">
@@ -5342,7 +5342,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="61">
@@ -5353,7 +5353,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="62">
@@ -5364,7 +5364,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="63">
@@ -5375,7 +5375,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="64">
@@ -5386,7 +5386,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="65">
@@ -5397,7 +5397,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="66">
@@ -5408,7 +5408,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="67">
@@ -5419,7 +5419,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="68">
@@ -5430,7 +5430,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="69">
@@ -5441,7 +5441,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="70">
@@ -5452,7 +5452,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="71">
@@ -5463,7 +5463,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="72">
@@ -5474,7 +5474,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="73">
@@ -5485,7 +5485,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="74">
@@ -5496,7 +5496,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="75">
@@ -5507,7 +5507,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="76">
@@ -5518,7 +5518,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="77">
@@ -5529,7 +5529,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="78">
@@ -5540,7 +5540,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="79">
@@ -5551,7 +5551,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="80">
@@ -5562,7 +5562,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="81">
@@ -5573,7 +5573,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="82">
@@ -5584,7 +5584,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="83">
@@ -5595,7 +5595,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="84">
@@ -5606,7 +5606,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="85">
@@ -5617,7 +5617,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="86">
@@ -5628,7 +5628,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="87">
@@ -5639,7 +5639,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="88">
@@ -5650,7 +5650,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="89">
@@ -5661,7 +5661,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="90">
@@ -5672,7 +5672,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="91">
@@ -5683,7 +5683,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>6773.035485</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="92">
@@ -5694,7 +5694,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>6773.035485</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="93">
@@ -5705,7 +5705,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="94">
@@ -5716,7 +5716,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>6773</v>
+        <v>39378.789999</v>
       </c>
     </row>
   </sheetData>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -5785,7 +5785,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>1178.593372</v>
+        <v>4729.841495</v>
       </c>
     </row>
     <row r="5">
@@ -5840,7 +5840,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>1040.674875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -5862,7 +5862,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>1458.802845</v>
+        <v>543.845569000001</v>
       </c>
     </row>
     <row r="12">
@@ -5873,7 +5873,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>121.404176</v>
+        <v>284.671257</v>
       </c>
     </row>
     <row r="13">
@@ -5884,7 +5884,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1721.494144</v>
       </c>
     </row>
     <row r="14">
@@ -5895,7 +5895,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>530.6550559999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -6368,7 +6368,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>2318.753089</v>
+        <v>1504.951812</v>
       </c>
     </row>
     <row r="58">
@@ -6522,7 +6522,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>1458.802845</v>
+        <v>695.9912660000009</v>
       </c>
     </row>
     <row r="72">
@@ -6533,7 +6533,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>174.0654459999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -6775,7 +6775,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>1392.055342</v>
+        <v>370.0158380000003</v>
       </c>
     </row>
   </sheetData>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -6822,7 +6822,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="3">
@@ -6833,7 +6833,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="4">
@@ -6844,7 +6844,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="5">
@@ -6855,7 +6855,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="6">
@@ -6866,7 +6866,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="7">
@@ -6877,7 +6877,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="8">
@@ -6888,7 +6888,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="9">
@@ -6899,7 +6899,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="10">
@@ -6910,7 +6910,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="11">
@@ -6921,7 +6921,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>4621.154430999999</v>
       </c>
     </row>
     <row r="12">
@@ -6932,7 +6932,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>4336.483173999999</v>
       </c>
     </row>
     <row r="13">
@@ -6943,7 +6943,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="14">
@@ -6954,7 +6954,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="15">
@@ -6965,7 +6965,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="16">
@@ -6976,7 +6976,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="17">
@@ -6987,7 +6987,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="18">
@@ -6998,7 +6998,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="19">
@@ -7009,7 +7009,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="20">
@@ -7020,7 +7020,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="21">
@@ -7031,7 +7031,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="22">
@@ -7042,7 +7042,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="23">
@@ -7053,7 +7053,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="24">
@@ -7064,7 +7064,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="25">
@@ -7075,7 +7075,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="26">
@@ -7086,7 +7086,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="27">
@@ -7097,7 +7097,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="28">
@@ -7108,7 +7108,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="29">
@@ -7119,7 +7119,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="30">
@@ -7130,7 +7130,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="31">
@@ -7141,7 +7141,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="32">
@@ -7152,7 +7152,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="33">
@@ -7163,7 +7163,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="34">
@@ -7174,7 +7174,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="35">
@@ -7185,7 +7185,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="36">
@@ -7196,7 +7196,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="37">
@@ -7207,7 +7207,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="38">
@@ -7218,7 +7218,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="39">
@@ -7229,7 +7229,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="40">
@@ -7240,7 +7240,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="41">
@@ -7251,7 +7251,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="42">
@@ -7262,7 +7262,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="43">
@@ -7273,7 +7273,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="44">
@@ -7284,7 +7284,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="45">
@@ -7295,7 +7295,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="46">
@@ -7306,7 +7306,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="47">
@@ -7317,7 +7317,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="48">
@@ -7328,7 +7328,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="49">
@@ -7339,7 +7339,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="50">
@@ -7350,7 +7350,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="51">
@@ -7361,7 +7361,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="52">
@@ -7372,7 +7372,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="53">
@@ -7383,7 +7383,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="54">
@@ -7394,7 +7394,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="55">
@@ -7405,7 +7405,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="56">
@@ -7416,7 +7416,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>2614.989029999999</v>
       </c>
     </row>
     <row r="57">
@@ -7427,7 +7427,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="58">
@@ -7438,7 +7438,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="59">
@@ -7449,7 +7449,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="60">
@@ -7460,7 +7460,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="61">
@@ -7471,7 +7471,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="62">
@@ -7482,7 +7482,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="63">
@@ -7493,7 +7493,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="64">
@@ -7504,7 +7504,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="65">
@@ -7515,7 +7515,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="66">
@@ -7526,7 +7526,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="67">
@@ -7537,7 +7537,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="68">
@@ -7548,7 +7548,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="69">
@@ -7559,7 +7559,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="70">
@@ -7570,7 +7570,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1110.037217999999</v>
       </c>
     </row>
     <row r="71">
@@ -7581,7 +7581,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="72">
@@ -7592,7 +7592,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="73">
@@ -7603,7 +7603,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="74">
@@ -7614,7 +7614,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="75">
@@ -7625,7 +7625,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="76">
@@ -7636,7 +7636,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="77">
@@ -7647,7 +7647,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="78">
@@ -7658,7 +7658,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="79">
@@ -7669,7 +7669,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="80">
@@ -7680,7 +7680,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="81">
@@ -7691,7 +7691,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="82">
@@ -7702,7 +7702,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="83">
@@ -7713,7 +7713,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="84">
@@ -7724,7 +7724,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="85">
@@ -7735,7 +7735,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="86">
@@ -7746,7 +7746,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="87">
@@ -7757,7 +7757,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="88">
@@ -7768,7 +7768,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="89">
@@ -7779,7 +7779,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="90">
@@ -7790,7 +7790,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="91">
@@ -7801,7 +7801,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="92">
@@ -7812,7 +7812,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="93">
@@ -7823,7 +7823,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>414.0459519999977</v>
       </c>
     </row>
     <row r="94">
@@ -7834,7 +7834,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>44.03011399999741</v>
       </c>
     </row>
   </sheetData>
@@ -7869,7 +7869,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -7903,7 +7903,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="5">
@@ -7980,7 +7980,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>543.845569000001</v>
       </c>
     </row>
     <row r="12">
@@ -7991,7 +7991,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>284.671257</v>
       </c>
     </row>
     <row r="13">
@@ -8002,7 +8002,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1721.494144</v>
       </c>
     </row>
     <row r="14">
@@ -8486,7 +8486,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1504.951812</v>
       </c>
     </row>
     <row r="58">
@@ -8640,7 +8640,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>695.9912660000009</v>
       </c>
     </row>
     <row r="72">
@@ -8893,7 +8893,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>370.0158380000003</v>
       </c>
     </row>
   </sheetData>
@@ -8928,7 +8928,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -9987,7 +9987,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -10021,7 +10021,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>1178.593372</v>
+        <v>3007.841495</v>
       </c>
     </row>
     <row r="5">
@@ -10076,7 +10076,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>1040.674875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -10098,7 +10098,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>1458.802845</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -10109,7 +10109,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>121.404176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -10131,7 +10131,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>530.6550559999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -10604,7 +10604,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>2318.753089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -10758,7 +10758,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>1458.802845</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -10769,7 +10769,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>174.0654459999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -11011,7 +11011,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>1392.055342</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11046,7 +11046,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>City of Coalinga</t>
+          <t>City of Tracy</t>
         </is>
       </c>
     </row>
@@ -11080,7 +11080,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>677.3035485</v>
+        <v>3007.841495</v>
       </c>
     </row>
     <row r="5">
@@ -11135,7 +11135,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>677.3000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -11157,7 +11157,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>677.3000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -11168,7 +11168,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>121.404176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -11190,7 +11190,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>530.6550559999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -11663,7 +11663,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>677.3000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -11817,7 +11817,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>677.3000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -11828,7 +11828,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>174.0654459999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -12070,7 +12070,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>677.3000000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed long-term WMO cost calcs. Subtracting groundwater pumping savings from reliability management cost as CWEST implemented.
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -446,7 +446,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total Annual Cost</t>
+          <t>Total Annual Cost ($)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -468,7 +468,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>74609684.54060502</v>
+        <v>86980252.17294382</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +501,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +534,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="9">
@@ -545,7 +545,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>34636862.16021674</v>
+        <v>46903868.62131204</v>
       </c>
     </row>
     <row r="10">
@@ -556,7 +556,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="11">
@@ -567,7 +567,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>34761233.58251005</v>
+        <v>88007049.22104913</v>
       </c>
     </row>
     <row r="12">
@@ -578,7 +578,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>34877823.78496338</v>
+        <v>88389183.98585439</v>
       </c>
     </row>
     <row r="13">
@@ -589,7 +589,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>35328480.30778956</v>
+        <v>85705228.6802958</v>
       </c>
     </row>
     <row r="14">
@@ -600,7 +600,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>34636862.16021674</v>
+        <v>87682647.45584138</v>
       </c>
     </row>
     <row r="15">
@@ -611,7 +611,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="16">
@@ -622,7 +622,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="17">
@@ -633,7 +633,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="18">
@@ -644,7 +644,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="19">
@@ -655,7 +655,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="20">
@@ -666,7 +666,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="22">
@@ -688,7 +688,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="23">
@@ -699,7 +699,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="24">
@@ -710,7 +710,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="25">
@@ -721,7 +721,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="27">
@@ -743,7 +743,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="28">
@@ -754,7 +754,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="29">
@@ -765,7 +765,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="30">
@@ -776,7 +776,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="31">
@@ -787,7 +787,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="32">
@@ -798,7 +798,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="33">
@@ -809,7 +809,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="34">
@@ -820,7 +820,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="35">
@@ -831,7 +831,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="36">
@@ -842,7 +842,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="37">
@@ -853,7 +853,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="38">
@@ -864,7 +864,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="39">
@@ -875,7 +875,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="40">
@@ -886,7 +886,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="41">
@@ -897,7 +897,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="42">
@@ -908,7 +908,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="43">
@@ -919,7 +919,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="45">
@@ -941,7 +941,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="46">
@@ -952,7 +952,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="48">
@@ -974,7 +974,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="49">
@@ -985,7 +985,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="50">
@@ -996,7 +996,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="51">
@@ -1007,7 +1007,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="52">
@@ -1018,7 +1018,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="53">
@@ -1029,7 +1029,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="54">
@@ -1040,7 +1040,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="55">
@@ -1051,7 +1051,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="56">
@@ -1062,7 +1062,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>34934793.77734198</v>
+        <v>87326238.0282841</v>
       </c>
     </row>
     <row r="57">
@@ -1073,7 +1073,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>34981027.87197478</v>
+        <v>85477789.148054</v>
       </c>
     </row>
     <row r="58">
@@ -1084,7 +1084,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="59">
@@ -1095,7 +1095,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="60">
@@ -1106,7 +1106,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="61">
@@ -1117,7 +1117,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="62">
@@ -1128,7 +1128,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="63">
@@ -1139,7 +1139,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="64">
@@ -1150,7 +1150,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="65">
@@ -1161,7 +1161,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="66">
@@ -1172,7 +1172,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="67">
@@ -1183,7 +1183,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="68">
@@ -1194,7 +1194,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="69">
@@ -1205,7 +1205,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="70">
@@ -1216,7 +1216,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="71">
@@ -1227,7 +1227,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>34796027.60825985</v>
+        <v>86121632.8870099</v>
       </c>
     </row>
     <row r="72">
@@ -1238,7 +1238,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="73">
@@ -1249,7 +1249,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="74">
@@ -1260,7 +1260,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="75">
@@ -1271,7 +1271,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="76">
@@ -1282,7 +1282,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="77">
@@ -1293,7 +1293,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="78">
@@ -1304,7 +1304,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="79">
@@ -1315,7 +1315,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="80">
@@ -1326,7 +1326,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="81">
@@ -1337,7 +1337,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="82">
@@ -1348,7 +1348,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="83">
@@ -1359,7 +1359,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="84">
@@ -1370,7 +1370,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="85">
@@ -1381,7 +1381,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="86">
@@ -1392,7 +1392,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="87">
@@ -1403,7 +1403,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="88">
@@ -1414,7 +1414,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="89">
@@ -1425,7 +1425,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="90">
@@ -1436,7 +1436,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="91">
@@ -1447,7 +1447,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>34812722.64019499</v>
+        <v>46708889.18421242</v>
       </c>
     </row>
     <row r="92">
@@ -1458,7 +1458,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>34934793.77734198</v>
+        <v>46830960.32135942</v>
       </c>
     </row>
     <row r="93">
@@ -1469,7 +1469,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>34636862.16021674</v>
+        <v>46533028.70423418</v>
       </c>
     </row>
     <row r="94">
@@ -1480,7 +1480,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>34721480.65978038</v>
+        <v>86381073.52278507</v>
       </c>
     </row>
   </sheetData>
@@ -1505,7 +1505,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Water Market Transfer Deliveries</t>
+          <t>Water Market Transfer Deliveries (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1549,7 +1549,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>995.4122350999983</v>
       </c>
     </row>
     <row r="5">
@@ -2564,7 +2564,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total Shortage</t>
+          <t>Total Shortage (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -3623,7 +3623,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total Economic Loss</t>
+          <t>Total Economic Loss ($)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -4682,7 +4682,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Applied Demands</t>
+          <t>Applied Demands (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -5741,7 +5741,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Demands to be met by storage</t>
+          <t>Demands to be met by storage (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -5785,7 +5785,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>4729.841495</v>
+        <v>6655.312234999999</v>
       </c>
     </row>
     <row r="5">
@@ -5840,7 +5840,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1621.591535999999</v>
       </c>
     </row>
     <row r="10">
@@ -5862,7 +5862,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>543.845569000001</v>
+        <v>2469.316309</v>
       </c>
     </row>
     <row r="12">
@@ -5873,7 +5873,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>284.671257</v>
+        <v>2210.141996999999</v>
       </c>
     </row>
     <row r="13">
@@ -5884,7 +5884,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>1721.494144</v>
+        <v>3646.964883999999</v>
       </c>
     </row>
     <row r="14">
@@ -5895,7 +5895,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>660.1177829999997</v>
       </c>
     </row>
     <row r="15">
@@ -6357,7 +6357,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1482.267718999998</v>
       </c>
     </row>
     <row r="57">
@@ -6368,7 +6368,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>1504.951812</v>
+        <v>3430.422551999999</v>
       </c>
     </row>
     <row r="58">
@@ -6522,7 +6522,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>695.9912660000009</v>
+        <v>2621.462006</v>
       </c>
     </row>
     <row r="72">
@@ -6775,7 +6775,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>370.0158380000003</v>
+        <v>2295.486577999999</v>
       </c>
     </row>
   </sheetData>
@@ -6800,7 +6800,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>GW bank volume</t>
+          <t>GW bank volume (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -6899,7 +6899,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>5165</v>
+        <v>3543.408464000001</v>
       </c>
     </row>
     <row r="10">
@@ -6910,7 +6910,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>5165</v>
+        <v>3543.408464000001</v>
       </c>
     </row>
     <row r="11">
@@ -6921,7 +6921,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>4621.154430999999</v>
+        <v>1821.408464000001</v>
       </c>
     </row>
     <row r="12">
@@ -6932,7 +6932,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>4336.483173999999</v>
+        <v>99.408464000001</v>
       </c>
     </row>
     <row r="13">
@@ -6943,7 +6943,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -6954,7 +6954,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -6965,7 +6965,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -6976,7 +6976,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -6987,7 +6987,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -6998,7 +6998,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -7009,7 +7009,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -7020,7 +7020,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -7031,7 +7031,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -7042,7 +7042,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -7053,7 +7053,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -7064,7 +7064,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -7075,7 +7075,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -7086,7 +7086,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -7097,7 +7097,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -7108,7 +7108,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -7119,7 +7119,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -7130,7 +7130,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -7141,7 +7141,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -7152,7 +7152,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -7163,7 +7163,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -7174,7 +7174,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -7185,7 +7185,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -7196,7 +7196,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -7207,7 +7207,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -7218,7 +7218,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -7229,7 +7229,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -7240,7 +7240,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -7251,7 +7251,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -7262,7 +7262,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -7273,7 +7273,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -7284,7 +7284,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -7295,7 +7295,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -7306,7 +7306,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -7317,7 +7317,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -7328,7 +7328,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -7339,7 +7339,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -7350,7 +7350,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -7361,7 +7361,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -7372,7 +7372,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -7383,7 +7383,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -7394,7 +7394,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -7405,7 +7405,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -7416,7 +7416,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>2614.989029999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -7427,7 +7427,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -7438,7 +7438,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -7449,7 +7449,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -7460,7 +7460,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -7471,7 +7471,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -7482,7 +7482,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -7493,7 +7493,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -7504,7 +7504,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -7515,7 +7515,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -7526,7 +7526,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -7537,7 +7537,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -7548,7 +7548,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -7559,7 +7559,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -7570,7 +7570,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>1110.037217999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -7581,7 +7581,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -7592,7 +7592,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -7603,7 +7603,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -7614,7 +7614,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -7625,7 +7625,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -7636,7 +7636,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -7647,7 +7647,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -7658,7 +7658,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -7669,7 +7669,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -7680,7 +7680,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -7691,7 +7691,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -7702,7 +7702,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -7713,7 +7713,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -7724,7 +7724,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -7735,7 +7735,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -7746,7 +7746,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -7757,7 +7757,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -7768,7 +7768,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -7779,7 +7779,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -7790,7 +7790,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -7801,7 +7801,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -7812,7 +7812,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -7823,7 +7823,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>414.0459519999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -7834,7 +7834,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>44.03011399999741</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7859,7 +7859,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>GW bank take volume</t>
+          <t>GW bank take volume (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -7958,7 +7958,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1621.591535999999</v>
       </c>
     </row>
     <row r="10">
@@ -7980,7 +7980,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>543.845569000001</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="12">
@@ -7991,7 +7991,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>284.671257</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="13">
@@ -8002,7 +8002,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>1721.494144</v>
+        <v>99.408464000001</v>
       </c>
     </row>
     <row r="14">
@@ -8486,7 +8486,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>1504.951812</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -8640,7 +8640,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>695.9912660000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -8893,7 +8893,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>370.0158380000003</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8918,7 +8918,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>GW bank put volume</t>
+          <t>GW bank put volume (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -9977,7 +9977,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Contingent Options Demands</t>
+          <t>Contingent Options Demands (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -10021,7 +10021,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>3007.841495</v>
+        <v>4933.312234999999</v>
       </c>
     </row>
     <row r="5">
@@ -10098,7 +10098,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>747.3163089999998</v>
       </c>
     </row>
     <row r="12">
@@ -10109,7 +10109,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>488.1419969999988</v>
       </c>
     </row>
     <row r="13">
@@ -10120,7 +10120,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>3547.556419999998</v>
       </c>
     </row>
     <row r="14">
@@ -10131,7 +10131,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>660.1177829999997</v>
       </c>
     </row>
     <row r="15">
@@ -10593,7 +10593,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1482.267718999998</v>
       </c>
     </row>
     <row r="57">
@@ -10604,7 +10604,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>3430.422551999999</v>
       </c>
     </row>
     <row r="58">
@@ -10758,7 +10758,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>2621.462006</v>
       </c>
     </row>
     <row r="72">
@@ -11011,7 +11011,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>2295.486577999999</v>
       </c>
     </row>
   </sheetData>
@@ -11036,7 +11036,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Contingent Conservation Volume</t>
+          <t>Contingent Conservation Volume (acre-feet/year)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -11080,7 +11080,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>3007.841495</v>
+        <v>3937.8999999</v>
       </c>
     </row>
     <row r="5">
@@ -11157,7 +11157,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>747.3163089999998</v>
       </c>
     </row>
     <row r="12">
@@ -11168,7 +11168,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>488.1419969999988</v>
       </c>
     </row>
     <row r="13">
@@ -11179,7 +11179,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>3547.556419999998</v>
       </c>
     </row>
     <row r="14">
@@ -11190,7 +11190,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>660.1177829999997</v>
       </c>
     </row>
     <row r="15">
@@ -11652,7 +11652,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1482.267718999998</v>
       </c>
     </row>
     <row r="57">
@@ -11663,7 +11663,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>3430.422551999999</v>
       </c>
     </row>
     <row r="58">
@@ -11817,7 +11817,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>2621.462006</v>
       </c>
     </row>
     <row r="72">
@@ -12070,7 +12070,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>2295.486577999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typo in puts into storage function
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -468,7 +468,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>46708889.18421242</v>
+        <v>45807729.61110652</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>46708889.18421242</v>
+        <v>42223064.90923876</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>86980252.17294382</v>
+        <v>167994658.2539075</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +501,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>46533028.70423418</v>
+        <v>43175548.81164407</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>46533028.70423418</v>
+        <v>41801572.39731208</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>46708889.18421242</v>
+        <v>41840035.23585714</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +534,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>46830960.32135942</v>
+        <v>41948366.60886081</v>
       </c>
     </row>
     <row r="9">
@@ -545,7 +545,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>46903868.62131204</v>
+        <v>82414291.77402699</v>
       </c>
     </row>
     <row r="10">
@@ -556,7 +556,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>46533028.70423418</v>
+        <v>42783610.50005091</v>
       </c>
     </row>
     <row r="11">
@@ -567,7 +567,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>88007049.22104913</v>
+        <v>81739595.96821465</v>
       </c>
     </row>
     <row r="12">
@@ -578,7 +578,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>88389183.98585439</v>
+        <v>82121730.7330199</v>
       </c>
     </row>
     <row r="13">
@@ -589,7 +589,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>85705228.6802958</v>
+        <v>81100248.67173503</v>
       </c>
     </row>
     <row r="14">
@@ -600,7 +600,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>87682647.45584138</v>
+        <v>83179519.273811</v>
       </c>
     </row>
     <row r="15">
@@ -611,7 +611,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>46708889.18421242</v>
+        <v>42124736.56246825</v>
       </c>
     </row>
     <row r="16">
@@ -622,7 +622,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>46708889.18421242</v>
+        <v>44694860.39210407</v>
       </c>
     </row>
     <row r="17">
@@ -633,7 +633,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>46708889.18421242</v>
+        <v>42512370.07678195</v>
       </c>
     </row>
     <row r="18">
@@ -644,7 +644,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>46708889.18421242</v>
+        <v>46168356.5368732</v>
       </c>
     </row>
     <row r="19">
@@ -655,7 +655,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>46830960.32135942</v>
+        <v>42099331.34319243</v>
       </c>
     </row>
     <row r="20">
@@ -666,7 +666,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>46708889.18421242</v>
+        <v>42834862.88937473</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>46708889.18421242</v>
+        <v>41925778.23706558</v>
       </c>
     </row>
     <row r="22">
@@ -688,7 +688,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>46708889.18421242</v>
+        <v>41834869.77183466</v>
       </c>
     </row>
     <row r="23">
@@ -699,7 +699,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>46708889.18421242</v>
+        <v>41825778.92531157</v>
       </c>
     </row>
     <row r="24">
@@ -710,7 +710,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>46830960.32135942</v>
+        <v>42296542.0332</v>
       </c>
     </row>
     <row r="25">
@@ -721,7 +721,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>46708889.18421242</v>
+        <v>43145179.39332803</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>46708889.18421242</v>
+        <v>41956809.8874609</v>
       </c>
     </row>
     <row r="27">
@@ -743,7 +743,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>46830960.32135942</v>
+        <v>42238351.4991427</v>
       </c>
     </row>
     <row r="28">
@@ -754,7 +754,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>46533028.70423418</v>
+        <v>42290813.95033397</v>
       </c>
     </row>
     <row r="29">
@@ -765,7 +765,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>46533028.70423418</v>
+        <v>42185007.04374775</v>
       </c>
     </row>
     <row r="30">
@@ -776,7 +776,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>46533028.70423418</v>
+        <v>41702518.22052246</v>
       </c>
     </row>
     <row r="31">
@@ -787,7 +787,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>46708889.18421242</v>
+        <v>41830129.81817818</v>
       </c>
     </row>
     <row r="32">
@@ -798,7 +798,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>46708889.18421242</v>
+        <v>41825304.92994592</v>
       </c>
     </row>
     <row r="33">
@@ -809,7 +809,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>46830960.32135942</v>
+        <v>41946893.57826969</v>
       </c>
     </row>
     <row r="34">
@@ -820,7 +820,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>46533028.70423418</v>
+        <v>41648913.71226212</v>
       </c>
     </row>
     <row r="35">
@@ -831,7 +831,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>46533028.70423418</v>
+        <v>41648908.88737389</v>
       </c>
     </row>
     <row r="36">
@@ -842,7 +842,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>46708889.18421242</v>
+        <v>41824768.88486332</v>
       </c>
     </row>
     <row r="37">
@@ -853,7 +853,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>46830960.32135942</v>
+        <v>42259587.12802847</v>
       </c>
     </row>
     <row r="38">
@@ -864,7 +864,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>46708889.18421242</v>
+        <v>43005554.15071774</v>
       </c>
     </row>
     <row r="39">
@@ -875,7 +875,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>46830960.32135942</v>
+        <v>42064918.50034688</v>
       </c>
     </row>
     <row r="40">
@@ -886,7 +886,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>46533028.70423418</v>
+        <v>41660716.20446984</v>
       </c>
     </row>
     <row r="41">
@@ -897,7 +897,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>46533028.70423418</v>
+        <v>41650089.13659466</v>
       </c>
     </row>
     <row r="42">
@@ -908,7 +908,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>46533028.70423418</v>
+        <v>41649026.42980714</v>
       </c>
     </row>
     <row r="43">
@@ -919,7 +919,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>46708889.18421242</v>
+        <v>41824780.63910664</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>46830960.32135942</v>
+        <v>42340056.31798558</v>
       </c>
     </row>
     <row r="45">
@@ -941,7 +941,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>46708889.18421242</v>
+        <v>43309368.91745385</v>
       </c>
     </row>
     <row r="46">
@@ -952,7 +952,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>46830960.32135942</v>
+        <v>42095299.97702048</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>46708889.18421242</v>
+        <v>41839614.83211545</v>
       </c>
     </row>
     <row r="48">
@@ -974,7 +974,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>46830960.32135942</v>
+        <v>41948324.56848664</v>
       </c>
     </row>
     <row r="49">
@@ -985,7 +985,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>46708889.18421242</v>
+        <v>41824917.29126206</v>
       </c>
     </row>
     <row r="50">
@@ -996,7 +996,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>46708889.18421242</v>
+        <v>41824783.6772543</v>
       </c>
     </row>
     <row r="51">
@@ -1007,7 +1007,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>46830960.32135942</v>
+        <v>41946841.45300052</v>
       </c>
     </row>
     <row r="52">
@@ -1018,7 +1018,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>46533028.70423418</v>
+        <v>41648908.49973521</v>
       </c>
     </row>
     <row r="53">
@@ -1029,7 +1029,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>46708889.18421242</v>
+        <v>41824768.84609945</v>
       </c>
     </row>
     <row r="54">
@@ -1040,7 +1040,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>46708889.18421242</v>
+        <v>41824768.83273804</v>
       </c>
     </row>
     <row r="55">
@@ -1051,7 +1051,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>46708889.18421242</v>
+        <v>41824768.83140191</v>
       </c>
     </row>
     <row r="56">
@@ -1062,7 +1062,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>87326238.0282841</v>
+        <v>82823109.84625371</v>
       </c>
     </row>
     <row r="57">
@@ -1073,7 +1073,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>85477789.148054</v>
+        <v>80974660.96602361</v>
       </c>
     </row>
     <row r="58">
@@ -1084,7 +1084,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>46708889.18421242</v>
+        <v>44798390.53640898</v>
       </c>
     </row>
     <row r="59">
@@ -1095,7 +1095,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>46708889.18421242</v>
+        <v>42122131.001769</v>
       </c>
     </row>
     <row r="60">
@@ -1106,7 +1106,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>46708889.18421242</v>
+        <v>41854505.048305</v>
       </c>
     </row>
     <row r="61">
@@ -1117,7 +1117,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>46830960.32135942</v>
+        <v>41949813.59010559</v>
       </c>
     </row>
     <row r="62">
@@ -1128,7 +1128,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>46708889.18421242</v>
+        <v>41825066.19342396</v>
       </c>
     </row>
     <row r="63">
@@ -1139,7 +1139,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>46708889.18421242</v>
+        <v>41824798.5674705</v>
       </c>
     </row>
     <row r="64">
@@ -1150,7 +1150,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>46708889.18421242</v>
+        <v>41824771.80487515</v>
       </c>
     </row>
     <row r="65">
@@ -1161,7 +1161,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>46830960.32135942</v>
+        <v>41946840.26576261</v>
       </c>
     </row>
     <row r="66">
@@ -1172,7 +1172,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>46708889.18421242</v>
+        <v>41824768.86098966</v>
       </c>
     </row>
     <row r="67">
@@ -1183,7 +1183,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>46830960.32135942</v>
+        <v>42212391.53578003</v>
       </c>
     </row>
     <row r="68">
@@ -1194,7 +1194,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>46533028.70423418</v>
+        <v>42054508.57407267</v>
       </c>
     </row>
     <row r="69">
@@ -1205,7 +1205,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>46533028.70423418</v>
+        <v>42123120.7418641</v>
       </c>
     </row>
     <row r="70">
@@ -1216,7 +1216,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>46533028.70423418</v>
+        <v>41811505.94180849</v>
       </c>
     </row>
     <row r="71">
@@ -1227,7 +1227,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>86121632.8870099</v>
+        <v>81618504.70497951</v>
       </c>
     </row>
     <row r="72">
@@ -1238,7 +1238,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>46533028.70423418</v>
+        <v>42002113.269846</v>
       </c>
     </row>
     <row r="73">
@@ -1249,7 +1249,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>46708889.18421242</v>
+        <v>45469771.66901121</v>
       </c>
     </row>
     <row r="74">
@@ -1260,7 +1260,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>46830960.32135942</v>
+        <v>42061237.59723587</v>
       </c>
     </row>
     <row r="75">
@@ -1271,7 +1271,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>46708889.18421242</v>
+        <v>42621180.44000424</v>
       </c>
     </row>
     <row r="76">
@@ -1282,7 +1282,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>46708889.18421242</v>
+        <v>41904409.99212853</v>
       </c>
     </row>
     <row r="77">
@@ -1293,7 +1293,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>46708889.18421242</v>
+        <v>41832732.94734095</v>
       </c>
     </row>
     <row r="78">
@@ -1304,7 +1304,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>46708889.18421242</v>
+        <v>41825565.24286219</v>
       </c>
     </row>
     <row r="79">
@@ -1315,7 +1315,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>46708889.18421242</v>
+        <v>41824848.47241432</v>
       </c>
     </row>
     <row r="80">
@@ -1326,7 +1326,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>46708889.18421242</v>
+        <v>41824776.79536954</v>
       </c>
     </row>
     <row r="81">
@@ -1337,7 +1337,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>46830960.32135942</v>
+        <v>42041849.86580111</v>
       </c>
     </row>
     <row r="82">
@@ -1348,7 +1348,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>46533028.70423418</v>
+        <v>42007621.57109812</v>
       </c>
     </row>
     <row r="83">
@@ -1359,7 +1359,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>46533028.70423418</v>
+        <v>41684779.67325749</v>
       </c>
     </row>
     <row r="84">
@@ -1370,7 +1370,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>46533028.70423418</v>
+        <v>41652495.48347343</v>
       </c>
     </row>
     <row r="85">
@@ -1381,7 +1381,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>46708889.18421242</v>
+        <v>41825127.54447327</v>
       </c>
     </row>
     <row r="86">
@@ -1392,7 +1392,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>46708889.18421242</v>
+        <v>41824804.70257543</v>
       </c>
     </row>
     <row r="87">
@@ -1403,7 +1403,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>46830960.32135942</v>
+        <v>41946843.55553263</v>
       </c>
     </row>
     <row r="88">
@@ -1414,7 +1414,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>46533028.70423418</v>
+        <v>41648908.70998842</v>
       </c>
     </row>
     <row r="89">
@@ -1425,7 +1425,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>46533028.70423418</v>
+        <v>41759655.07385854</v>
       </c>
     </row>
     <row r="90">
@@ -1436,7 +1436,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>46708889.18421242</v>
+        <v>42242896.09733533</v>
       </c>
     </row>
     <row r="91">
@@ -1447,7 +1447,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>46708889.18421242</v>
+        <v>41866581.55786163</v>
       </c>
     </row>
     <row r="92">
@@ -1458,7 +1458,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>46830960.32135942</v>
+        <v>41951021.24106126</v>
       </c>
     </row>
     <row r="93">
@@ -1469,7 +1469,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>46533028.70423418</v>
+        <v>41649326.47854128</v>
       </c>
     </row>
     <row r="94">
@@ -1480,7 +1480,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>86381073.52278507</v>
+        <v>81877945.34075467</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1549,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>995.4122350999983</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
@@ -2608,7 +2608,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1733.5074751</v>
       </c>
     </row>
     <row r="5">
@@ -3667,7 +3667,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>3922609.877851271</v>
       </c>
     </row>
     <row r="5">
@@ -5785,7 +5785,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>6655.312234999999</v>
+        <v>8393.407475</v>
       </c>
     </row>
     <row r="5">
@@ -5840,7 +5840,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>1621.591535999999</v>
+        <v>3359.686776</v>
       </c>
     </row>
     <row r="10">
@@ -5862,7 +5862,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>2469.316309</v>
+        <v>4207.411549</v>
       </c>
     </row>
     <row r="12">
@@ -5873,7 +5873,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>2210.141996999999</v>
+        <v>3948.237236999999</v>
       </c>
     </row>
     <row r="13">
@@ -5884,7 +5884,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>3646.964883999999</v>
+        <v>5385.060124</v>
       </c>
     </row>
     <row r="14">
@@ -5895,7 +5895,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>660.1177829999997</v>
+        <v>2398.213023</v>
       </c>
     </row>
     <row r="15">
@@ -5906,7 +5906,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1311.684939000001</v>
       </c>
     </row>
     <row r="16">
@@ -5950,7 +5950,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>666.8071889999992</v>
       </c>
     </row>
     <row r="20">
@@ -6005,7 +6005,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1529.160919</v>
       </c>
     </row>
     <row r="25">
@@ -6038,7 +6038,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1274.708058999999</v>
       </c>
     </row>
     <row r="28">
@@ -6148,7 +6148,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1367.566228999998</v>
       </c>
     </row>
     <row r="38">
@@ -6225,7 +6225,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1719.438158999999</v>
       </c>
     </row>
     <row r="45">
@@ -6357,7 +6357,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>1482.267718999998</v>
+        <v>3220.362958999998</v>
       </c>
     </row>
     <row r="57">
@@ -6368,7 +6368,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3430.422551999999</v>
+        <v>5168.517792</v>
       </c>
     </row>
     <row r="58">
@@ -6478,7 +6478,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1161.191538999999</v>
       </c>
     </row>
     <row r="68">
@@ -6511,7 +6511,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>710.9991790000004</v>
       </c>
     </row>
     <row r="71">
@@ -6522,7 +6522,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>2621.462006</v>
+        <v>4359.557246</v>
       </c>
     </row>
     <row r="72">
@@ -6533,7 +6533,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1544.478035</v>
       </c>
     </row>
     <row r="73">
@@ -6555,7 +6555,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>500.2326289999983</v>
       </c>
     </row>
     <row r="75">
@@ -6632,7 +6632,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>415.4548589999995</v>
       </c>
     </row>
     <row r="82">
@@ -6720,7 +6720,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>484.2681159999993</v>
       </c>
     </row>
     <row r="90">
@@ -6775,7 +6775,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>2295.486577999999</v>
+        <v>4033.581818</v>
       </c>
     </row>
   </sheetData>
@@ -6822,7 +6822,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>6887</v>
+        <v>11038.7</v>
       </c>
     </row>
     <row r="3">
@@ -6833,7 +6833,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>6887</v>
+        <v>11453.87</v>
       </c>
     </row>
     <row r="4">
@@ -6844,7 +6844,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>5165</v>
+        <v>9731.870000000001</v>
       </c>
     </row>
     <row r="5">
@@ -6855,7 +6855,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>5165</v>
+        <v>11323.187</v>
       </c>
     </row>
     <row r="6">
@@ -6866,7 +6866,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>5165</v>
+        <v>11482.3187</v>
       </c>
     </row>
     <row r="7">
@@ -6877,7 +6877,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>5165</v>
+        <v>11498.23187</v>
       </c>
     </row>
     <row r="8">
@@ -6888,7 +6888,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>5165</v>
+        <v>11499.823187</v>
       </c>
     </row>
     <row r="9">
@@ -6899,7 +6899,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>3543.408464000001</v>
+        <v>9777.823187</v>
       </c>
     </row>
     <row r="10">
@@ -6910,7 +6910,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>3543.408464000001</v>
+        <v>10960.5973019</v>
       </c>
     </row>
     <row r="11">
@@ -6921,7 +6921,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>1821.408464000001</v>
+        <v>9238.597301900001</v>
       </c>
     </row>
     <row r="12">
@@ -6932,7 +6932,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>99.408464000001</v>
+        <v>7516.597301900001</v>
       </c>
     </row>
     <row r="13">
@@ -6943,7 +6943,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>5794.597301900001</v>
       </c>
     </row>
     <row r="14">
@@ -6954,7 +6954,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>4072.597301900001</v>
       </c>
     </row>
     <row r="15">
@@ -6965,7 +6965,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2760.912362900001</v>
       </c>
     </row>
     <row r="16">
@@ -6976,7 +6976,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>5752.596135800001</v>
       </c>
     </row>
     <row r="17">
@@ -6987,7 +6987,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>6469.327795700002</v>
       </c>
     </row>
     <row r="18">
@@ -6998,7 +6998,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>10996.93277957</v>
       </c>
     </row>
     <row r="19">
@@ -7009,7 +7009,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>10330.12559057</v>
       </c>
     </row>
     <row r="20">
@@ -7020,7 +7020,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>11383.012559057</v>
       </c>
     </row>
     <row r="21">
@@ -7031,7 +7031,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>11488.3012559057</v>
       </c>
     </row>
     <row r="22">
@@ -7042,7 +7042,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>11498.83012559057</v>
       </c>
     </row>
     <row r="23">
@@ -7053,7 +7053,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>11499.88301255906</v>
       </c>
     </row>
     <row r="24">
@@ -7064,7 +7064,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>9970.722093559058</v>
       </c>
     </row>
     <row r="25">
@@ -7075,7 +7075,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>11347.07220935591</v>
       </c>
     </row>
     <row r="26">
@@ -7086,7 +7086,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>11484.70722093559</v>
       </c>
     </row>
     <row r="27">
@@ -7097,7 +7097,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>10209.99916193559</v>
       </c>
     </row>
     <row r="28">
@@ -7108,7 +7108,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>10879.09926683559</v>
       </c>
     </row>
     <row r="29">
@@ -7119,7 +7119,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>11437.90992668356</v>
       </c>
     </row>
     <row r="30">
@@ -7130,7 +7130,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>11493.79099266836</v>
       </c>
     </row>
     <row r="31">
@@ -7141,7 +7141,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>11499.37909926684</v>
       </c>
     </row>
     <row r="32">
@@ -7152,7 +7152,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>11499.93790992668</v>
       </c>
     </row>
     <row r="33">
@@ -7163,7 +7163,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>11499.99379099267</v>
       </c>
     </row>
     <row r="34">
@@ -7174,7 +7174,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>11499.99937909927</v>
       </c>
     </row>
     <row r="35">
@@ -7185,7 +7185,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>11499.99993790993</v>
       </c>
     </row>
     <row r="36">
@@ -7196,7 +7196,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>11499.99999379099</v>
       </c>
     </row>
     <row r="37">
@@ -7207,7 +7207,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>10132.43376479099</v>
       </c>
     </row>
     <row r="38">
@@ -7218,7 +7218,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>11363.2433764791</v>
       </c>
     </row>
     <row r="39">
@@ -7229,7 +7229,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>11486.32433764791</v>
       </c>
     </row>
     <row r="40">
@@ -7240,7 +7240,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>11498.63243376479</v>
       </c>
     </row>
     <row r="41">
@@ -7251,7 +7251,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>11499.86324337648</v>
       </c>
     </row>
     <row r="42">
@@ -7262,7 +7262,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>11499.98632433765</v>
       </c>
     </row>
     <row r="43">
@@ -7273,7 +7273,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>11499.99863243376</v>
       </c>
     </row>
     <row r="44">
@@ -7284,7 +7284,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>9780.560473433765</v>
       </c>
     </row>
     <row r="45">
@@ -7295,7 +7295,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>11328.05604734338</v>
       </c>
     </row>
     <row r="46">
@@ -7306,7 +7306,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>11482.80560473434</v>
       </c>
     </row>
     <row r="47">
@@ -7317,7 +7317,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>11498.28056047343</v>
       </c>
     </row>
     <row r="48">
@@ -7328,7 +7328,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>11499.82805604734</v>
       </c>
     </row>
     <row r="49">
@@ -7339,7 +7339,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>11499.98280560473</v>
       </c>
     </row>
     <row r="50">
@@ -7350,7 +7350,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>11499.99828056047</v>
       </c>
     </row>
     <row r="51">
@@ -7361,7 +7361,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>11499.99982805605</v>
       </c>
     </row>
     <row r="52">
@@ -7372,7 +7372,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>11499.9999828056</v>
       </c>
     </row>
     <row r="53">
@@ -7383,7 +7383,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>11499.99999828056</v>
       </c>
     </row>
     <row r="54">
@@ -7394,7 +7394,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>11499.99999982806</v>
       </c>
     </row>
     <row r="55">
@@ -7405,7 +7405,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>11499.99999998281</v>
       </c>
     </row>
     <row r="56">
@@ -7416,7 +7416,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>9777.999999982805</v>
       </c>
     </row>
     <row r="57">
@@ -7427,7 +7427,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>8055.999999982805</v>
       </c>
     </row>
     <row r="58">
@@ -7438,7 +7438,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>11155.59999999828</v>
       </c>
     </row>
     <row r="59">
@@ -7449,7 +7449,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>11465.55999999983</v>
       </c>
     </row>
     <row r="60">
@@ -7460,7 +7460,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>11496.55599999998</v>
       </c>
     </row>
     <row r="61">
@@ -7471,7 +7471,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>11499.6556</v>
       </c>
     </row>
     <row r="62">
@@ -7482,7 +7482,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>11499.96556</v>
       </c>
     </row>
     <row r="63">
@@ -7493,7 +7493,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>11499.996556</v>
       </c>
     </row>
     <row r="64">
@@ -7504,7 +7504,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>11499.9996556</v>
       </c>
     </row>
     <row r="65">
@@ -7515,7 +7515,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>11499.99996556</v>
       </c>
     </row>
     <row r="66">
@@ -7526,7 +7526,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>11499.999996556</v>
       </c>
     </row>
     <row r="67">
@@ -7537,7 +7537,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>10338.808457556</v>
       </c>
     </row>
     <row r="68">
@@ -7548,7 +7548,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>10761.592044456</v>
       </c>
     </row>
     <row r="69">
@@ -7559,7 +7559,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>11255.894572356</v>
       </c>
     </row>
     <row r="70">
@@ -7570,7 +7570,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>10544.895393356</v>
       </c>
     </row>
     <row r="71">
@@ -7581,7 +7581,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>8822.895393355999</v>
       </c>
     </row>
     <row r="72">
@@ -7592,7 +7592,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>7278.417358355999</v>
       </c>
     </row>
     <row r="73">
@@ -7603,7 +7603,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>11077.8417358356</v>
       </c>
     </row>
     <row r="74">
@@ -7614,7 +7614,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>10577.6091068356</v>
       </c>
     </row>
     <row r="75">
@@ -7625,7 +7625,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>11407.76091068356</v>
       </c>
     </row>
     <row r="76">
@@ -7636,7 +7636,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>11490.77609106836</v>
       </c>
     </row>
     <row r="77">
@@ -7647,7 +7647,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>11499.07760910684</v>
       </c>
     </row>
     <row r="78">
@@ -7658,7 +7658,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>11499.90776091068</v>
       </c>
     </row>
     <row r="79">
@@ -7669,7 +7669,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>11499.99077609107</v>
       </c>
     </row>
     <row r="80">
@@ -7680,7 +7680,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>11499.99907760911</v>
       </c>
     </row>
     <row r="81">
@@ -7691,7 +7691,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>11084.54421860911</v>
       </c>
     </row>
     <row r="82">
@@ -7702,7 +7702,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>11458.45442186091</v>
       </c>
     </row>
     <row r="83">
@@ -7713,7 +7713,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>11495.84544218609</v>
       </c>
     </row>
     <row r="84">
@@ -7724,7 +7724,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>11499.58454421861</v>
       </c>
     </row>
     <row r="85">
@@ -7735,7 +7735,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>11499.95845442186</v>
       </c>
     </row>
     <row r="86">
@@ -7746,7 +7746,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>11499.99584544219</v>
       </c>
     </row>
     <row r="87">
@@ -7757,7 +7757,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>11499.99958454422</v>
       </c>
     </row>
     <row r="88">
@@ -7768,7 +7768,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>11499.99995845442</v>
       </c>
     </row>
     <row r="89">
@@ -7779,7 +7779,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>11015.73184245442</v>
       </c>
     </row>
     <row r="90">
@@ -7790,7 +7790,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>11451.57318424544</v>
       </c>
     </row>
     <row r="91">
@@ -7801,7 +7801,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>11495.15731842454</v>
       </c>
     </row>
     <row r="92">
@@ -7812,7 +7812,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>11499.51573184245</v>
       </c>
     </row>
     <row r="93">
@@ -7823,7 +7823,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>11499.95157318425</v>
       </c>
     </row>
     <row r="94">
@@ -7834,7 +7834,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>9777.951573184246</v>
       </c>
     </row>
   </sheetData>
@@ -7958,7 +7958,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>1621.591535999999</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="10">
@@ -8002,7 +8002,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>99.408464000001</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="14">
@@ -8013,7 +8013,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="15">
@@ -8024,7 +8024,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1311.684939000001</v>
       </c>
     </row>
     <row r="16">
@@ -8068,7 +8068,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>666.8071889999992</v>
       </c>
     </row>
     <row r="20">
@@ -8123,7 +8123,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1529.160919</v>
       </c>
     </row>
     <row r="25">
@@ -8156,7 +8156,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1274.708058999999</v>
       </c>
     </row>
     <row r="28">
@@ -8266,7 +8266,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1367.566228999998</v>
       </c>
     </row>
     <row r="38">
@@ -8343,7 +8343,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1719.438158999999</v>
       </c>
     </row>
     <row r="45">
@@ -8475,7 +8475,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="57">
@@ -8486,7 +8486,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="58">
@@ -8596,7 +8596,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>1161.191538999999</v>
       </c>
     </row>
     <row r="68">
@@ -8629,7 +8629,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>710.9991790000004</v>
       </c>
     </row>
     <row r="71">
@@ -8640,7 +8640,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="72">
@@ -8651,7 +8651,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1544.478035</v>
       </c>
     </row>
     <row r="73">
@@ -8673,7 +8673,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>500.2326289999983</v>
       </c>
     </row>
     <row r="75">
@@ -8750,7 +8750,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>415.4548589999995</v>
       </c>
     </row>
     <row r="82">
@@ -8838,7 +8838,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>484.2681159999993</v>
       </c>
     </row>
     <row r="90">
@@ -8893,7 +8893,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
   </sheetData>
@@ -8940,7 +8940,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4151.7</v>
       </c>
     </row>
     <row r="3">
@@ -8951,7 +8951,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>415.1699999999993</v>
       </c>
     </row>
     <row r="4">
@@ -8973,7 +8973,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1591.316999999999</v>
       </c>
     </row>
     <row r="6">
@@ -8984,7 +8984,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>159.1317000000001</v>
       </c>
     </row>
     <row r="7">
@@ -8995,7 +8995,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>15.91317000000017</v>
       </c>
     </row>
     <row r="8">
@@ -9006,7 +9006,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1.591317000000345</v>
       </c>
     </row>
     <row r="9">
@@ -9028,7 +9028,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1182.774114900001</v>
       </c>
     </row>
     <row r="11">
@@ -9094,7 +9094,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>2991.683772900001</v>
       </c>
     </row>
     <row r="17">
@@ -9105,7 +9105,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>716.7316599000005</v>
       </c>
     </row>
     <row r="18">
@@ -9116,7 +9116,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>4527.604983869998</v>
       </c>
     </row>
     <row r="19">
@@ -9138,7 +9138,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1052.886968486999</v>
       </c>
     </row>
     <row r="21">
@@ -9149,7 +9149,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>105.2886968486995</v>
       </c>
     </row>
     <row r="22">
@@ -9160,7 +9160,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>10.52886968486946</v>
       </c>
     </row>
     <row r="23">
@@ -9171,7 +9171,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1.05288696848711</v>
       </c>
     </row>
     <row r="24">
@@ -9193,7 +9193,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1376.350115796848</v>
       </c>
     </row>
     <row r="26">
@@ -9204,7 +9204,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>137.6350115796853</v>
       </c>
     </row>
     <row r="27">
@@ -9226,7 +9226,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>669.1001049000002</v>
       </c>
     </row>
     <row r="29">
@@ -9237,7 +9237,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>558.8106598479671</v>
       </c>
     </row>
     <row r="30">
@@ -9248,7 +9248,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>55.88106598479754</v>
       </c>
     </row>
     <row r="31">
@@ -9259,7 +9259,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>5.588106598480408</v>
       </c>
     </row>
     <row r="32">
@@ -9270,7 +9270,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.5588106598472223</v>
       </c>
     </row>
     <row r="33">
@@ -9281,7 +9281,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.05588106598406739</v>
       </c>
     </row>
     <row r="34">
@@ -9292,7 +9292,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.005588106598406739</v>
       </c>
     </row>
     <row r="35">
@@ -9303,7 +9303,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>0.0005588106600043829</v>
       </c>
     </row>
     <row r="36">
@@ -9314,7 +9314,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>5.588106632785639e-05</v>
       </c>
     </row>
     <row r="37">
@@ -9336,7 +9336,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1230.809611688105</v>
       </c>
     </row>
     <row r="39">
@@ -9347,7 +9347,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>123.0809611688113</v>
       </c>
     </row>
     <row r="40">
@@ -9358,7 +9358,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>12.30809611688146</v>
       </c>
     </row>
     <row r="41">
@@ -9369,7 +9369,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1.230809611687983</v>
       </c>
     </row>
     <row r="42">
@@ -9380,7 +9380,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.1230809611683071</v>
       </c>
     </row>
     <row r="43">
@@ -9391,7 +9391,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.01230809611715813</v>
       </c>
     </row>
     <row r="44">
@@ -9413,7 +9413,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1547.495573909612</v>
       </c>
     </row>
     <row r="46">
@@ -9424,7 +9424,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>154.7495573909615</v>
       </c>
     </row>
     <row r="47">
@@ -9435,7 +9435,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>15.47495573909582</v>
       </c>
     </row>
     <row r="48">
@@ -9446,7 +9446,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1.547495573910237</v>
       </c>
     </row>
     <row r="49">
@@ -9457,7 +9457,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>0.1547495573911874</v>
       </c>
     </row>
     <row r="50">
@@ -9468,7 +9468,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>0.01547495573977358</v>
       </c>
     </row>
     <row r="51">
@@ -9479,7 +9479,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>0.001547495573322521</v>
       </c>
     </row>
     <row r="52">
@@ -9490,7 +9490,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>0.0001547495579870883</v>
       </c>
     </row>
     <row r="53">
@@ -9501,7 +9501,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1.547495612612693e-05</v>
       </c>
     </row>
     <row r="54">
@@ -9512,7 +9512,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1.547495776321739e-06</v>
       </c>
     </row>
     <row r="55">
@@ -9523,7 +9523,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>1.547492502140813e-07</v>
       </c>
     </row>
     <row r="56">
@@ -9556,7 +9556,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>3099.600000015475</v>
       </c>
     </row>
     <row r="59">
@@ -9567,7 +9567,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>309.9600000015467</v>
       </c>
     </row>
     <row r="60">
@@ -9578,7 +9578,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>30.99600000015435</v>
       </c>
     </row>
     <row r="61">
@@ -9589,7 +9589,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>3.099600000015926</v>
       </c>
     </row>
     <row r="62">
@@ -9600,7 +9600,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>0.3099600000015926</v>
       </c>
     </row>
     <row r="63">
@@ -9611,7 +9611,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>0.03099599999950442</v>
       </c>
     </row>
     <row r="64">
@@ -9622,7 +9622,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>0.003099599999950442</v>
       </c>
     </row>
     <row r="65">
@@ -9633,7 +9633,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>0.0003099599995039171</v>
       </c>
     </row>
     <row r="66">
@@ -9644,7 +9644,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>3.099599962297361e-05</v>
       </c>
     </row>
     <row r="67">
@@ -9666,7 +9666,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>422.7835868999995</v>
       </c>
     </row>
     <row r="69">
@@ -9677,7 +9677,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>494.3025279</v>
       </c>
     </row>
     <row r="70">
@@ -9721,7 +9721,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>3799.424377479601</v>
       </c>
     </row>
     <row r="74">
@@ -9743,7 +9743,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>830.1518038479584</v>
       </c>
     </row>
     <row r="76">
@@ -9754,7 +9754,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>83.01518038479536</v>
       </c>
     </row>
     <row r="77">
@@ -9765,7 +9765,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>8.301518038480026</v>
       </c>
     </row>
     <row r="78">
@@ -9776,7 +9776,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>0.8301518038471841</v>
       </c>
     </row>
     <row r="79">
@@ -9787,7 +9787,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>0.08301518038406357</v>
       </c>
     </row>
     <row r="80">
@@ -9798,7 +9798,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>0.008301518038570066</v>
       </c>
     </row>
     <row r="81">
@@ -9820,7 +9820,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>373.9102032518031</v>
       </c>
     </row>
     <row r="83">
@@ -9831,7 +9831,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>37.39102032517949</v>
       </c>
     </row>
     <row r="84">
@@ -9842,7 +9842,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>3.739102032517621</v>
       </c>
     </row>
     <row r="85">
@@ -9853,7 +9853,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>0.3739102032517622</v>
       </c>
     </row>
     <row r="86">
@@ -9864,7 +9864,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>0.03739102032468509</v>
       </c>
     </row>
     <row r="87">
@@ -9875,7 +9875,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>0.003739102031977381</v>
       </c>
     </row>
     <row r="88">
@@ -9886,7 +9886,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>0.0003739102028703201</v>
       </c>
     </row>
     <row r="89">
@@ -9908,7 +9908,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>435.8413417910195</v>
       </c>
     </row>
     <row r="91">
@@ -9919,7 +9919,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>43.58413417910179</v>
       </c>
     </row>
     <row r="92">
@@ -9930,7 +9930,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>4.358413417910015</v>
       </c>
     </row>
     <row r="93">
@@ -9941,7 +9941,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>0.43584134179182</v>
       </c>
     </row>
     <row r="94">
@@ -10021,7 +10021,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>4933.312234999999</v>
+        <v>6671.407475</v>
       </c>
     </row>
     <row r="5">
@@ -10076,7 +10076,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1637.686776</v>
       </c>
     </row>
     <row r="10">
@@ -10098,7 +10098,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>747.3163089999998</v>
+        <v>2485.411549</v>
       </c>
     </row>
     <row r="12">
@@ -10109,7 +10109,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>488.1419969999988</v>
+        <v>2226.237236999999</v>
       </c>
     </row>
     <row r="13">
@@ -10120,7 +10120,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>3547.556419999998</v>
+        <v>3663.060124</v>
       </c>
     </row>
     <row r="14">
@@ -10131,7 +10131,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>660.1177829999997</v>
+        <v>676.2130230000002</v>
       </c>
     </row>
     <row r="15">
@@ -10593,7 +10593,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>1482.267718999998</v>
+        <v>1498.362958999998</v>
       </c>
     </row>
     <row r="57">
@@ -10604,7 +10604,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3430.422551999999</v>
+        <v>3446.517792</v>
       </c>
     </row>
     <row r="58">
@@ -10758,7 +10758,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>2621.462006</v>
+        <v>2637.557246</v>
       </c>
     </row>
     <row r="72">
@@ -11011,7 +11011,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>2295.486577999999</v>
+        <v>2311.581818</v>
       </c>
     </row>
   </sheetData>
@@ -11135,7 +11135,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1637.686776</v>
       </c>
     </row>
     <row r="10">
@@ -11157,7 +11157,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>747.3163089999998</v>
+        <v>2485.411549</v>
       </c>
     </row>
     <row r="12">
@@ -11168,7 +11168,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>488.1419969999988</v>
+        <v>2226.237236999999</v>
       </c>
     </row>
     <row r="13">
@@ -11179,7 +11179,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>3547.556419999998</v>
+        <v>3663.060124</v>
       </c>
     </row>
     <row r="14">
@@ -11190,7 +11190,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>660.1177829999997</v>
+        <v>676.2130230000002</v>
       </c>
     </row>
     <row r="15">
@@ -11652,7 +11652,7 @@
         <v>1976</v>
       </c>
       <c r="C56" t="n">
-        <v>1482.267718999998</v>
+        <v>1498.362958999998</v>
       </c>
     </row>
     <row r="57">
@@ -11663,7 +11663,7 @@
         <v>1977</v>
       </c>
       <c r="C57" t="n">
-        <v>3430.422551999999</v>
+        <v>3446.517792</v>
       </c>
     </row>
     <row r="58">
@@ -11817,7 +11817,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>2621.462006</v>
+        <v>2637.557246</v>
       </c>
     </row>
     <row r="72">
@@ -12070,7 +12070,7 @@
         <v>2014</v>
       </c>
       <c r="C94" t="n">
-        <v>2295.486577999999</v>
+        <v>2311.581818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typo in puts into storage test
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -468,7 +468,7 @@
         <v>1922</v>
       </c>
       <c r="C2" t="n">
-        <v>45807729.61110652</v>
+        <v>42136288.29979742</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>42223064.90923876</v>
+        <v>41855920.77810784</v>
       </c>
     </row>
     <row r="4">
@@ -501,7 +501,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>43175548.81164407</v>
+        <v>41768311.54180558</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>41801572.39731208</v>
+        <v>41660848.67032823</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>41840035.23585714</v>
+        <v>41825962.86315875</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +534,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>41948366.60886081</v>
+        <v>41946959.37159097</v>
       </c>
     </row>
     <row r="9">
@@ -556,7 +556,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>42783610.50005091</v>
+        <v>41737656.85518473</v>
       </c>
     </row>
     <row r="11">
@@ -622,7 +622,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>44694860.39210407</v>
+        <v>42049247.41568523</v>
       </c>
     </row>
     <row r="17">
@@ -633,7 +633,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>42512370.07678195</v>
+        <v>41878548.21458574</v>
       </c>
     </row>
     <row r="18">
@@ -644,7 +644,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>46168356.5368732</v>
+        <v>42164494.02776385</v>
       </c>
     </row>
     <row r="19">
@@ -666,7 +666,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>42834862.88937473</v>
+        <v>41903771.35765467</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>41925778.23706558</v>
+        <v>41832669.08389357</v>
       </c>
     </row>
     <row r="22">
@@ -688,7 +688,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>41834869.77183466</v>
+        <v>41825558.85651746</v>
       </c>
     </row>
     <row r="23">
@@ -699,7 +699,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>41825778.92531157</v>
+        <v>41824847.83377985</v>
       </c>
     </row>
     <row r="24">
@@ -721,7 +721,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>43145179.39332803</v>
+        <v>41928042.1546158</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>41956809.8874609</v>
+        <v>41835096.16358968</v>
       </c>
     </row>
     <row r="27">
@@ -754,7 +754,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>42290813.95033397</v>
+        <v>41699113.73920813</v>
       </c>
     </row>
     <row r="29">
@@ -765,7 +765,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>42185007.04374775</v>
+        <v>41690838.25945077</v>
       </c>
     </row>
     <row r="30">
@@ -776,7 +776,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>41702518.22052246</v>
+        <v>41653101.34209275</v>
       </c>
     </row>
     <row r="31">
@@ -787,7 +787,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>41830129.81817818</v>
+        <v>41825188.1303352</v>
       </c>
     </row>
     <row r="32">
@@ -798,7 +798,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>41825304.92994592</v>
+        <v>41824810.76116162</v>
       </c>
     </row>
     <row r="33">
@@ -809,7 +809,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>41946893.57826969</v>
+        <v>41946844.16139126</v>
       </c>
     </row>
     <row r="34">
@@ -820,7 +820,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>41648913.71226212</v>
+        <v>41648908.77057428</v>
       </c>
     </row>
     <row r="35">
@@ -831,7 +831,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>41648908.88737389</v>
+        <v>41648908.39320511</v>
       </c>
     </row>
     <row r="36">
@@ -842,7 +842,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>41824768.88486332</v>
+        <v>41824768.83544643</v>
       </c>
     </row>
     <row r="37">
@@ -864,7 +864,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>43005554.15071774</v>
+        <v>41917121.64000935</v>
       </c>
     </row>
     <row r="39">
@@ -875,7 +875,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>42064918.50034688</v>
+        <v>41956075.24927603</v>
       </c>
     </row>
     <row r="40">
@@ -886,7 +886,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>41660716.20446984</v>
+        <v>41649831.87936275</v>
       </c>
     </row>
     <row r="41">
@@ -897,7 +897,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>41650089.13659466</v>
+        <v>41649000.70408395</v>
       </c>
     </row>
     <row r="42">
@@ -908,7 +908,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>41649026.42980714</v>
+        <v>41648917.58655607</v>
       </c>
     </row>
     <row r="43">
@@ -919,7 +919,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>41824780.63910664</v>
+        <v>41824769.75478153</v>
       </c>
     </row>
     <row r="44">
@@ -941,7 +941,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>43309368.91745385</v>
+        <v>41940883.91634111</v>
       </c>
     </row>
     <row r="46">
@@ -952,7 +952,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>42095299.97702048</v>
+        <v>41958451.47690921</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>41839614.83211545</v>
+        <v>41825929.98210432</v>
       </c>
     </row>
     <row r="48">
@@ -974,7 +974,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>41948324.56848664</v>
+        <v>41946956.08348553</v>
       </c>
     </row>
     <row r="49">
@@ -985,7 +985,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>41824917.29126206</v>
+        <v>41824780.44276195</v>
       </c>
     </row>
     <row r="50">
@@ -996,7 +996,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>41824783.6772543</v>
+        <v>41824769.9924043</v>
       </c>
     </row>
     <row r="51">
@@ -1007,7 +1007,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>41946841.45300052</v>
+        <v>41946840.08451553</v>
       </c>
     </row>
     <row r="52">
@@ -1018,7 +1018,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>41648908.49973521</v>
+        <v>41648908.3628867</v>
       </c>
     </row>
     <row r="53">
@@ -1029,7 +1029,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>41824768.84609945</v>
+        <v>41824768.8324146</v>
       </c>
     </row>
     <row r="54">
@@ -1040,7 +1040,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>41824768.83273804</v>
+        <v>41824768.83136956</v>
       </c>
     </row>
     <row r="55">
@@ -1051,7 +1051,7 @@
         <v>1975</v>
       </c>
       <c r="C55" t="n">
-        <v>41824768.83140191</v>
+        <v>41824768.83126505</v>
       </c>
     </row>
     <row r="56">
@@ -1084,7 +1084,7 @@
         <v>1978</v>
       </c>
       <c r="C58" t="n">
-        <v>44798390.53640898</v>
+        <v>42057344.82294449</v>
       </c>
     </row>
     <row r="59">
@@ -1095,7 +1095,7 @@
         <v>1979</v>
       </c>
       <c r="C59" t="n">
-        <v>42122131.001769</v>
+        <v>41848026.43042255</v>
       </c>
     </row>
     <row r="60">
@@ -1106,7 +1106,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>41854505.048305</v>
+        <v>41827094.59117036</v>
       </c>
     </row>
     <row r="61">
@@ -1117,7 +1117,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>41949813.59010559</v>
+        <v>41947072.54439213</v>
       </c>
     </row>
     <row r="62">
@@ -1128,7 +1128,7 @@
         <v>1982</v>
       </c>
       <c r="C62" t="n">
-        <v>41825066.19342396</v>
+        <v>41824792.08885261</v>
       </c>
     </row>
     <row r="63">
@@ -1139,7 +1139,7 @@
         <v>1983</v>
       </c>
       <c r="C63" t="n">
-        <v>41824798.5674705</v>
+        <v>41824771.15701336</v>
       </c>
     </row>
     <row r="64">
@@ -1150,7 +1150,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>41824771.80487515</v>
+        <v>41824769.06382944</v>
       </c>
     </row>
     <row r="65">
@@ -1161,7 +1161,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>41946840.26576261</v>
+        <v>41946839.99165804</v>
       </c>
     </row>
     <row r="66">
@@ -1172,7 +1172,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>41824768.86098966</v>
+        <v>41824768.8335792</v>
       </c>
     </row>
     <row r="67">
@@ -1194,7 +1194,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>42054508.57407267</v>
+        <v>41680631.57749583</v>
       </c>
     </row>
     <row r="69">
@@ -1205,7 +1205,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>42123120.7418641</v>
+        <v>41685997.94368104</v>
       </c>
     </row>
     <row r="70">
@@ -1249,7 +1249,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>45469771.66901121</v>
+        <v>42109855.58194485</v>
       </c>
     </row>
     <row r="74">
@@ -1271,7 +1271,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>42621180.44000424</v>
+        <v>41887058.60381541</v>
       </c>
     </row>
     <row r="76">
@@ -1282,7 +1282,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>41904409.99212853</v>
+        <v>41830997.80850964</v>
       </c>
     </row>
     <row r="77">
@@ -1293,7 +1293,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>41832732.94734095</v>
+        <v>41825391.72897907</v>
       </c>
     </row>
     <row r="78">
@@ -1304,7 +1304,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>41825565.24286219</v>
+        <v>41824831.12102601</v>
       </c>
     </row>
     <row r="79">
@@ -1315,7 +1315,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>41824848.47241432</v>
+        <v>41824775.0602307</v>
       </c>
     </row>
     <row r="80">
@@ -1326,7 +1326,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>41824776.79536954</v>
+        <v>41824769.45415117</v>
       </c>
     </row>
     <row r="81">
@@ -1348,7 +1348,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>42007621.57109812</v>
+        <v>41676964.40248317</v>
       </c>
     </row>
     <row r="83">
@@ -1359,7 +1359,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>41684779.67325749</v>
+        <v>41651713.95639599</v>
       </c>
     </row>
     <row r="84">
@@ -1370,7 +1370,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>41652495.48347343</v>
+        <v>41649188.91178727</v>
       </c>
     </row>
     <row r="85">
@@ -1381,7 +1381,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>41825127.54447327</v>
+        <v>41824796.88730466</v>
       </c>
     </row>
     <row r="86">
@@ -1392,7 +1392,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>41824804.70257543</v>
+        <v>41824771.63685857</v>
       </c>
     </row>
     <row r="87">
@@ -1403,7 +1403,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>41946843.55553263</v>
+        <v>41946840.24896096</v>
       </c>
     </row>
     <row r="88">
@@ -1414,7 +1414,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>41648908.70998842</v>
+        <v>41648908.37933125</v>
       </c>
     </row>
     <row r="89">
@@ -1436,7 +1436,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>42242896.09733533</v>
+        <v>41857471.83560449</v>
       </c>
     </row>
     <row r="91">
@@ -1447,7 +1447,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>41866581.55786163</v>
+        <v>41828039.13168855</v>
       </c>
     </row>
     <row r="92">
@@ -1458,7 +1458,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>41951021.24106126</v>
+        <v>41947166.99844395</v>
       </c>
     </row>
     <row r="93">
@@ -1469,7 +1469,7 @@
         <v>2013</v>
       </c>
       <c r="C93" t="n">
-        <v>41649326.47854128</v>
+        <v>41648941.05427954</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
Updated hydrology input data.
</commit_message>
<xml_diff>
--- a/CaUWMET/Results_QAQC.xlsx
+++ b/CaUWMET/Results_QAQC.xlsx
@@ -479,7 +479,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>41855920.77810784</v>
+        <v>41977991.91525484</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>167994658.2539075</v>
+        <v>82185464.83759691</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +501,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>41768311.54180558</v>
+        <v>41834111.74048327</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>41660848.67032823</v>
+        <v>42292874.99134813</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>41825962.86315875</v>
+        <v>42037945.96587037</v>
       </c>
     </row>
     <row r="8">
@@ -534,7 +534,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>41946959.37159097</v>
+        <v>41968157.68186213</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>82121730.7330199</v>
+        <v>41910811.34754464</v>
       </c>
     </row>
     <row r="13">
@@ -589,7 +589,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>81100248.67173503</v>
+        <v>41795006.25678951</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>42124736.56246825</v>
+        <v>41749618.01423517</v>
       </c>
     </row>
     <row r="16">
@@ -622,7 +622,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>42049247.41568523</v>
+        <v>41949872.56347131</v>
       </c>
     </row>
     <row r="17">
@@ -633,7 +633,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>41878548.21458574</v>
+        <v>41854865.25247306</v>
       </c>
     </row>
     <row r="18">
@@ -644,7 +644,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>42164494.02776385</v>
+        <v>41827778.47337541</v>
       </c>
     </row>
     <row r="19">
@@ -666,7 +666,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>41903771.35765467</v>
+        <v>41694239.32223757</v>
       </c>
     </row>
     <row r="21">
@@ -677,7 +677,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>41832669.08389357</v>
+        <v>41829301.92834968</v>
       </c>
     </row>
     <row r="22">
@@ -688,7 +688,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>41825558.85651746</v>
+        <v>41825222.14096307</v>
       </c>
     </row>
     <row r="23">
@@ -699,7 +699,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>41824847.83377985</v>
+        <v>41946885.29937141</v>
       </c>
     </row>
     <row r="24">
@@ -710,7 +710,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>42296542.0332</v>
+        <v>41648912.88437229</v>
       </c>
     </row>
     <row r="25">
@@ -721,7 +721,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>41928042.1546158</v>
+        <v>41648908.80458491</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>41835096.16358968</v>
+        <v>41648908.39660617</v>
       </c>
     </row>
     <row r="27">
@@ -743,7 +743,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>42238351.4991427</v>
+        <v>41648908.3558083</v>
       </c>
     </row>
     <row r="28">
@@ -754,7 +754,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>41699113.73920813</v>
+        <v>83624913.99274127</v>
       </c>
     </row>
     <row r="29">
@@ -765,7 +765,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>41690838.25945077</v>
+        <v>41987331.42498541</v>
       </c>
     </row>
     <row r="30">
@@ -776,7 +776,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>41653101.34209275</v>
+        <v>41728754.03664698</v>
       </c>
     </row>
     <row r="31">
@@ -787,7 +787,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>41825188.1303352</v>
+        <v>41656892.91981237</v>
       </c>
     </row>
     <row r="32">
@@ -798,7 +798,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>41824810.76116162</v>
+        <v>41649706.80812892</v>
       </c>
     </row>
     <row r="33">
@@ -809,7 +809,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>41946844.16139126</v>
+        <v>41648988.19696057</v>
       </c>
     </row>
     <row r="34">
@@ -820,7 +820,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>41648908.77057428</v>
+        <v>41648916.33584373</v>
       </c>
     </row>
     <row r="35">
@@ -831,7 +831,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>41648908.39320511</v>
+        <v>41648909.14973205</v>
       </c>
     </row>
     <row r="36">
@@ -842,7 +842,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>41824768.83544643</v>
+        <v>41648908.43112088</v>
       </c>
     </row>
     <row r="37">
@@ -853,7 +853,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>42259587.12802847</v>
+        <v>41824768.83923801</v>
       </c>
     </row>
     <row r="38">
@@ -864,7 +864,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>41917121.64000935</v>
+        <v>41946839.9691989</v>
       </c>
     </row>
     <row r="39">
@@ -875,7 +875,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>41956075.24927603</v>
+        <v>41648908.35135504</v>
       </c>
     </row>
     <row r="40">
@@ -886,7 +886,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>41649831.87936275</v>
+        <v>41648908.35128318</v>
       </c>
     </row>
     <row r="41">
@@ -897,7 +897,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>41649000.70408395</v>
+        <v>41648908.351276</v>
       </c>
     </row>
     <row r="42">
@@ -908,7 +908,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>41648917.58655607</v>
+        <v>41648908.35127527</v>
       </c>
     </row>
     <row r="43">
@@ -919,7 +919,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>41824769.75478153</v>
+        <v>41824768.83125345</v>
       </c>
     </row>
     <row r="44">
@@ -941,7 +941,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>41940883.91634111</v>
+        <v>41765023.34401006</v>
       </c>
     </row>
     <row r="46">
@@ -952,7 +952,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>41958451.47690921</v>
+        <v>41660519.85054868</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>41825929.98210432</v>
+        <v>41825929.98118079</v>
       </c>
     </row>
     <row r="48">
@@ -974,7 +974,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>41946956.08348553</v>
+        <v>41824884.94624618</v>
       </c>
     </row>
     <row r="49">
@@ -985,7 +985,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>41824780.44276195</v>
+        <v>41946851.57989971</v>
       </c>
     </row>
     <row r="50">
@@ -996,7 +996,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>41824769.9924043</v>
+        <v>41648909.51242512</v>
       </c>
     </row>
     <row r="51">
@@ -1007,7 +1007,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>41946840.08451553</v>
+        <v>41648908.46739019</v>
       </c>
     </row>
     <row r="52">
@@ -1040,7 +1040,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>41824768.83136956</v>
+        <v>41946839.96851656</v>
       </c>
     </row>
     <row r="55">
@@ -1106,7 +1106,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>41827094.59117036</v>
+        <v>41949165.72831735</v>
       </c>
     </row>
     <row r="61">
@@ -1117,7 +1117,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>41947072.54439213</v>
+        <v>41825001.40724514</v>
       </c>
     </row>
     <row r="62">
@@ -1150,7 +1150,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>41824769.06382944</v>
+        <v>41946840.20097643</v>
       </c>
     </row>
     <row r="65">
@@ -1161,7 +1161,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>41946839.99165804</v>
+        <v>41648908.3745328</v>
       </c>
     </row>
     <row r="66">
@@ -1172,7 +1172,7 @@
         <v>1986</v>
       </c>
       <c r="C66" t="n">
-        <v>41824768.8335792</v>
+        <v>41648908.35360096</v>
       </c>
     </row>
     <row r="67">
@@ -1183,7 +1183,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>42212391.53578003</v>
+        <v>41824768.83148602</v>
       </c>
     </row>
     <row r="68">
@@ -1194,7 +1194,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>41680631.57749583</v>
+        <v>81982580.19616544</v>
       </c>
     </row>
     <row r="69">
@@ -1249,7 +1249,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>42109855.58194485</v>
+        <v>42116547.56843557</v>
       </c>
     </row>
     <row r="74">
@@ -1271,7 +1271,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>41887058.60381541</v>
+        <v>41947458.54978263</v>
       </c>
     </row>
     <row r="76">
@@ -1282,7 +1282,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>41830997.80850964</v>
+        <v>41959108.94025336</v>
       </c>
     </row>
     <row r="77">
@@ -1293,7 +1293,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>41825391.72897907</v>
+        <v>41650135.24846049</v>
       </c>
     </row>
     <row r="78">
@@ -1304,7 +1304,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>41824831.12102601</v>
+        <v>41824891.52097198</v>
       </c>
     </row>
     <row r="79">
@@ -1315,7 +1315,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>41824775.0602307</v>
+        <v>41946852.23737229</v>
       </c>
     </row>
     <row r="80">
@@ -1326,7 +1326,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>41824769.45415117</v>
+        <v>41824770.05815063</v>
       </c>
     </row>
     <row r="81">
@@ -1348,7 +1348,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>41676964.40248317</v>
+        <v>41676964.46288312</v>
       </c>
     </row>
     <row r="83">
@@ -1359,7 +1359,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>41651713.95639599</v>
+        <v>41651713.96243599</v>
       </c>
     </row>
     <row r="84">
@@ -1370,7 +1370,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>41649188.91178727</v>
+        <v>41649188.91239128</v>
       </c>
     </row>
     <row r="85">
@@ -1381,7 +1381,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>41824796.88730466</v>
+        <v>41824796.88736505</v>
       </c>
     </row>
     <row r="86">
@@ -1392,7 +1392,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>41824771.63685857</v>
+        <v>41824771.6368646</v>
       </c>
     </row>
     <row r="87">
@@ -1403,7 +1403,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>41946840.24896096</v>
+        <v>41946840.24896156</v>
       </c>
     </row>
     <row r="88">
@@ -1414,7 +1414,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>41648908.37933125</v>
+        <v>41648908.37933131</v>
       </c>
     </row>
     <row r="89">
@@ -1436,7 +1436,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>41857471.83560449</v>
+        <v>41857471.8356045</v>
       </c>
     </row>
     <row r="91">
@@ -1549,7 +1549,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2608,7 +2608,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>1733.5074751</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3667,7 +3667,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>3922609.877851271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -4715,7 +4715,7 @@
         <v>1923</v>
       </c>
       <c r="C3" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="4">
@@ -4726,7 +4726,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="5">
@@ -4748,7 +4748,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="7">
@@ -4825,7 +4825,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="14">
@@ -4935,7 +4935,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="24">
@@ -4946,7 +4946,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="25">
@@ -4979,7 +4979,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="28">
@@ -5001,7 +5001,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="30">
@@ -5045,7 +5045,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="34">
@@ -5089,7 +5089,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="38">
@@ -5100,7 +5100,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="39">
@@ -5111,7 +5111,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="40">
@@ -5188,7 +5188,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="47">
@@ -5210,7 +5210,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="49">
@@ -5221,7 +5221,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="50">
@@ -5243,7 +5243,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="52">
@@ -5276,7 +5276,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="55">
@@ -5342,7 +5342,7 @@
         <v>1980</v>
       </c>
       <c r="C60" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="61">
@@ -5353,7 +5353,7 @@
         <v>1981</v>
       </c>
       <c r="C61" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="62">
@@ -5386,7 +5386,7 @@
         <v>1984</v>
       </c>
       <c r="C64" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="65">
@@ -5397,7 +5397,7 @@
         <v>1985</v>
       </c>
       <c r="C65" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="66">
@@ -5419,7 +5419,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>39378.999999</v>
+        <v>39378.789999</v>
       </c>
     </row>
     <row r="68">
@@ -5430,7 +5430,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="69">
@@ -5518,7 +5518,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="77">
@@ -5551,7 +5551,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>39378.789999</v>
+        <v>39378.999999</v>
       </c>
     </row>
     <row r="80">
@@ -5785,7 +5785,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>8393.407475</v>
+        <v>3647.197475</v>
       </c>
     </row>
     <row r="5">
@@ -5807,7 +5807,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1513.125848999998</v>
       </c>
     </row>
     <row r="7">
@@ -5873,7 +5873,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>3948.237236999999</v>
+        <v>1145.237236999999</v>
       </c>
     </row>
     <row r="13">
@@ -5884,7 +5884,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>5385.060124</v>
+        <v>638.8501240000005</v>
       </c>
     </row>
     <row r="14">
@@ -5906,7 +5906,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>1311.684939000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -6005,7 +6005,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>1529.160919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -6038,7 +6038,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>1274.708058999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -6049,7 +6049,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>2059.555439</v>
       </c>
     </row>
     <row r="29">
@@ -6148,7 +6148,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>1367.566228999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -6478,7 +6478,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>1161.191538999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -6489,7 +6489,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>4276.450459</v>
       </c>
     </row>
     <row r="69">
@@ -6855,7 +6855,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>11323.187</v>
+        <v>9856.3853519</v>
       </c>
     </row>
     <row r="6">
@@ -6866,7 +6866,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>11482.3187</v>
+        <v>8343.259502900002</v>
       </c>
     </row>
     <row r="7">
@@ -6877,7 +6877,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>11498.23187</v>
+        <v>11184.32595029</v>
       </c>
     </row>
     <row r="8">
@@ -6888,7 +6888,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>11499.823187</v>
+        <v>11468.432595029</v>
       </c>
     </row>
     <row r="9">
@@ -6899,7 +6899,7 @@
         <v>1929</v>
       </c>
       <c r="C9" t="n">
-        <v>9777.823187</v>
+        <v>9746.432595029</v>
       </c>
     </row>
     <row r="10">
@@ -6910,7 +6910,7 @@
         <v>1930</v>
       </c>
       <c r="C10" t="n">
-        <v>10960.5973019</v>
+        <v>10929.206709929</v>
       </c>
     </row>
     <row r="11">
@@ -6921,7 +6921,7 @@
         <v>1931</v>
       </c>
       <c r="C11" t="n">
-        <v>9238.597301900001</v>
+        <v>9207.206709929002</v>
       </c>
     </row>
     <row r="12">
@@ -6932,7 +6932,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>7516.597301900001</v>
+        <v>8061.969472929002</v>
       </c>
     </row>
     <row r="13">
@@ -6943,7 +6943,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>5794.597301900001</v>
+        <v>7423.119348929002</v>
       </c>
     </row>
     <row r="14">
@@ -6954,7 +6954,7 @@
         <v>1934</v>
       </c>
       <c r="C14" t="n">
-        <v>4072.597301900001</v>
+        <v>5701.119348929002</v>
       </c>
     </row>
     <row r="15">
@@ -6965,7 +6965,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>2760.912362900001</v>
+        <v>7043.302903829001</v>
       </c>
     </row>
     <row r="16">
@@ -6976,7 +6976,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>5752.596135800001</v>
+        <v>11054.3302903829</v>
       </c>
     </row>
     <row r="17">
@@ -6987,7 +6987,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>6469.327795700002</v>
+        <v>11455.43302903829</v>
       </c>
     </row>
     <row r="18">
@@ -6998,7 +6998,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>10996.93277957</v>
+        <v>11495.54330290383</v>
       </c>
     </row>
     <row r="19">
@@ -7009,7 +7009,7 @@
         <v>1939</v>
       </c>
       <c r="C19" t="n">
-        <v>10330.12559057</v>
+        <v>10828.73611390383</v>
       </c>
     </row>
     <row r="20">
@@ -7020,7 +7020,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>11383.012559057</v>
+        <v>11432.87361139038</v>
       </c>
     </row>
     <row r="21">
@@ -7031,7 +7031,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>11488.3012559057</v>
+        <v>11493.28736113904</v>
       </c>
     </row>
     <row r="22">
@@ -7042,7 +7042,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>11498.83012559057</v>
+        <v>11499.3287361139</v>
       </c>
     </row>
     <row r="23">
@@ -7053,7 +7053,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>11499.88301255906</v>
+        <v>11499.93287361139</v>
       </c>
     </row>
     <row r="24">
@@ -7064,7 +7064,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>9970.722093559058</v>
+        <v>11499.99328736114</v>
       </c>
     </row>
     <row r="25">
@@ -7075,7 +7075,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>11347.07220935591</v>
+        <v>11499.99932873611</v>
       </c>
     </row>
     <row r="26">
@@ -7086,7 +7086,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>11484.70722093559</v>
+        <v>11499.99993287361</v>
       </c>
     </row>
     <row r="27">
@@ -7097,7 +7097,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>10209.99916193559</v>
+        <v>11499.99999328736</v>
       </c>
     </row>
     <row r="28">
@@ -7108,7 +7108,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>10879.09926683559</v>
+        <v>9777.999993287362</v>
       </c>
     </row>
     <row r="29">
@@ -7119,7 +7119,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>11437.90992668356</v>
+        <v>10317.64003918736</v>
       </c>
     </row>
     <row r="30">
@@ -7130,7 +7130,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>11493.79099266836</v>
+        <v>11381.76400391874</v>
       </c>
     </row>
     <row r="31">
@@ -7141,7 +7141,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>11499.37909926684</v>
+        <v>11488.17640039187</v>
       </c>
     </row>
     <row r="32">
@@ -7152,7 +7152,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>11499.93790992668</v>
+        <v>11498.81764003919</v>
       </c>
     </row>
     <row r="33">
@@ -7163,7 +7163,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>11499.99379099267</v>
+        <v>11499.88176400392</v>
       </c>
     </row>
     <row r="34">
@@ -7174,7 +7174,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>11499.99937909927</v>
+        <v>11499.98817640039</v>
       </c>
     </row>
     <row r="35">
@@ -7185,7 +7185,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>11499.99993790993</v>
+        <v>11499.99881764004</v>
       </c>
     </row>
     <row r="36">
@@ -7196,7 +7196,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>11499.99999379099</v>
+        <v>11499.999881764</v>
       </c>
     </row>
     <row r="37">
@@ -7207,7 +7207,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>10132.43376479099</v>
+        <v>11499.9999881764</v>
       </c>
     </row>
     <row r="38">
@@ -7218,7 +7218,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>11363.2433764791</v>
+        <v>11499.99999881764</v>
       </c>
     </row>
     <row r="39">
@@ -7229,7 +7229,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>11486.32433764791</v>
+        <v>11499.99999988176</v>
       </c>
     </row>
     <row r="40">
@@ -7240,7 +7240,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>11498.63243376479</v>
+        <v>11499.99999998818</v>
       </c>
     </row>
     <row r="41">
@@ -7251,7 +7251,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>11499.86324337648</v>
+        <v>11499.99999999882</v>
       </c>
     </row>
     <row r="42">
@@ -7262,7 +7262,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>11499.98632433765</v>
+        <v>11499.99999999988</v>
       </c>
     </row>
     <row r="43">
@@ -7273,7 +7273,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>11499.99863243376</v>
+        <v>11499.99999999999</v>
       </c>
     </row>
     <row r="44">
@@ -7284,7 +7284,7 @@
         <v>1964</v>
       </c>
       <c r="C44" t="n">
-        <v>9780.560473433765</v>
+        <v>9780.56184099999</v>
       </c>
     </row>
     <row r="45">
@@ -7295,7 +7295,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>11328.05604734338</v>
+        <v>11328.0561841</v>
       </c>
     </row>
     <row r="46">
@@ -7306,7 +7306,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>11482.80560473434</v>
+        <v>11482.80561841</v>
       </c>
     </row>
     <row r="47">
@@ -7317,7 +7317,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>11498.28056047343</v>
+        <v>11498.280561841</v>
       </c>
     </row>
     <row r="48">
@@ -7328,7 +7328,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>11499.82805604734</v>
+        <v>11499.8280561841</v>
       </c>
     </row>
     <row r="49">
@@ -7339,7 +7339,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>11499.98280560473</v>
+        <v>11499.98280561841</v>
       </c>
     </row>
     <row r="50">
@@ -7350,7 +7350,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>11499.99828056047</v>
+        <v>11499.99828056184</v>
       </c>
     </row>
     <row r="51">
@@ -7361,7 +7361,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>11499.99982805605</v>
+        <v>11499.99982805618</v>
       </c>
     </row>
     <row r="52">
@@ -7372,7 +7372,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>11499.9999828056</v>
+        <v>11499.99998280562</v>
       </c>
     </row>
     <row r="53">
@@ -7537,7 +7537,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>10338.808457556</v>
+        <v>11499.9999996556</v>
       </c>
     </row>
     <row r="68">
@@ -7548,7 +7548,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>10761.592044456</v>
+        <v>9777.9999996556</v>
       </c>
     </row>
     <row r="69">
@@ -7559,7 +7559,7 @@
         <v>1989</v>
       </c>
       <c r="C69" t="n">
-        <v>11255.894572356</v>
+        <v>10272.3025275556</v>
       </c>
     </row>
     <row r="70">
@@ -7570,7 +7570,7 @@
         <v>1990</v>
       </c>
       <c r="C70" t="n">
-        <v>10544.895393356</v>
+        <v>9561.303348555599</v>
       </c>
     </row>
     <row r="71">
@@ -7581,7 +7581,7 @@
         <v>1991</v>
       </c>
       <c r="C71" t="n">
-        <v>8822.895393355999</v>
+        <v>7839.303348555599</v>
       </c>
     </row>
     <row r="72">
@@ -7592,7 +7592,7 @@
         <v>1992</v>
       </c>
       <c r="C72" t="n">
-        <v>7278.417358355999</v>
+        <v>6294.825313555599</v>
       </c>
     </row>
     <row r="73">
@@ -7603,7 +7603,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>11077.8417358356</v>
+        <v>10183.4355144556</v>
       </c>
     </row>
     <row r="74">
@@ -7614,7 +7614,7 @@
         <v>1994</v>
       </c>
       <c r="C74" t="n">
-        <v>10577.6091068356</v>
+        <v>9683.202885455599</v>
       </c>
     </row>
     <row r="75">
@@ -7625,7 +7625,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>11407.76091068356</v>
+        <v>11318.32028854556</v>
       </c>
     </row>
     <row r="76">
@@ -7636,7 +7636,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>11490.77609106836</v>
+        <v>11481.83202885456</v>
       </c>
     </row>
     <row r="77">
@@ -7647,7 +7647,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>11499.07760910684</v>
+        <v>11498.18320288546</v>
       </c>
     </row>
     <row r="78">
@@ -7658,7 +7658,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>11499.90776091068</v>
+        <v>11499.81832028854</v>
       </c>
     </row>
     <row r="79">
@@ -7669,7 +7669,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>11499.99077609107</v>
+        <v>11499.98183202885</v>
       </c>
     </row>
     <row r="80">
@@ -7680,7 +7680,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>11499.99907760911</v>
+        <v>11499.99818320289</v>
       </c>
     </row>
     <row r="81">
@@ -7691,7 +7691,7 @@
         <v>2001</v>
       </c>
       <c r="C81" t="n">
-        <v>11084.54421860911</v>
+        <v>11084.54332420289</v>
       </c>
     </row>
     <row r="82">
@@ -7702,7 +7702,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>11458.45442186091</v>
+        <v>11458.45433242029</v>
       </c>
     </row>
     <row r="83">
@@ -7713,7 +7713,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>11495.84544218609</v>
+        <v>11495.84543324203</v>
       </c>
     </row>
     <row r="84">
@@ -7724,7 +7724,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>11499.58454421861</v>
+        <v>11499.5845433242</v>
       </c>
     </row>
     <row r="85">
@@ -7735,7 +7735,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>11499.95845442186</v>
+        <v>11499.95845433242</v>
       </c>
     </row>
     <row r="86">
@@ -7746,7 +7746,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>11499.99584544219</v>
+        <v>11499.99584543324</v>
       </c>
     </row>
     <row r="87">
@@ -7757,7 +7757,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>11499.99958454422</v>
+        <v>11499.99958454332</v>
       </c>
     </row>
     <row r="88">
@@ -7768,7 +7768,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>11499.99995845442</v>
+        <v>11499.99995845433</v>
       </c>
     </row>
     <row r="89">
@@ -7779,7 +7779,7 @@
         <v>2009</v>
       </c>
       <c r="C89" t="n">
-        <v>11015.73184245442</v>
+        <v>11015.73184245433</v>
       </c>
     </row>
     <row r="90">
@@ -7790,7 +7790,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>11451.57318424544</v>
+        <v>11451.57318424543</v>
       </c>
     </row>
     <row r="91">
@@ -7925,7 +7925,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1513.125848999998</v>
       </c>
     </row>
     <row r="7">
@@ -7991,7 +7991,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>1722</v>
+        <v>1145.237236999999</v>
       </c>
     </row>
     <row r="13">
@@ -8002,7 +8002,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>1722</v>
+        <v>638.8501240000005</v>
       </c>
     </row>
     <row r="14">
@@ -8024,7 +8024,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>1311.684939000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -8123,7 +8123,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>1529.160919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -8156,7 +8156,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>1274.708058999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -8167,7 +8167,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="29">
@@ -8266,7 +8266,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>1367.566228999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -8596,7 +8596,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>1161.191538999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -8607,7 +8607,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="69">
@@ -8973,7 +8973,7 @@
         <v>1925</v>
       </c>
       <c r="C5" t="n">
-        <v>1591.316999999999</v>
+        <v>124.5153519</v>
       </c>
     </row>
     <row r="6">
@@ -8984,7 +8984,7 @@
         <v>1926</v>
       </c>
       <c r="C6" t="n">
-        <v>159.1317000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -8995,7 +8995,7 @@
         <v>1927</v>
       </c>
       <c r="C7" t="n">
-        <v>15.91317000000017</v>
+        <v>2841.066447389998</v>
       </c>
     </row>
     <row r="8">
@@ -9006,7 +9006,7 @@
         <v>1928</v>
       </c>
       <c r="C8" t="n">
-        <v>1.591317000000345</v>
+        <v>284.106644739</v>
       </c>
     </row>
     <row r="9">
@@ -9083,7 +9083,7 @@
         <v>1935</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1342.1835549</v>
       </c>
     </row>
     <row r="16">
@@ -9094,7 +9094,7 @@
         <v>1936</v>
       </c>
       <c r="C16" t="n">
-        <v>2991.683772900001</v>
+        <v>4011.027386553899</v>
       </c>
     </row>
     <row r="17">
@@ -9105,7 +9105,7 @@
         <v>1937</v>
       </c>
       <c r="C17" t="n">
-        <v>716.7316599000005</v>
+        <v>401.1027386553893</v>
       </c>
     </row>
     <row r="18">
@@ -9116,7 +9116,7 @@
         <v>1938</v>
       </c>
       <c r="C18" t="n">
-        <v>4527.604983869998</v>
+        <v>40.11027386553942</v>
       </c>
     </row>
     <row r="19">
@@ -9138,7 +9138,7 @@
         <v>1940</v>
       </c>
       <c r="C20" t="n">
-        <v>1052.886968486999</v>
+        <v>604.1374974865536</v>
       </c>
     </row>
     <row r="21">
@@ -9149,7 +9149,7 @@
         <v>1941</v>
       </c>
       <c r="C21" t="n">
-        <v>105.2886968486995</v>
+        <v>60.41374974865503</v>
       </c>
     </row>
     <row r="22">
@@ -9160,7 +9160,7 @@
         <v>1942</v>
       </c>
       <c r="C22" t="n">
-        <v>10.52886968486946</v>
+        <v>6.041374974865175</v>
       </c>
     </row>
     <row r="23">
@@ -9171,7 +9171,7 @@
         <v>1943</v>
       </c>
       <c r="C23" t="n">
-        <v>1.05288696848711</v>
+        <v>0.6041374974858628</v>
       </c>
     </row>
     <row r="24">
@@ -9182,7 +9182,7 @@
         <v>1944</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.06041374974793143</v>
       </c>
     </row>
     <row r="25">
@@ -9193,7 +9193,7 @@
         <v>1945</v>
       </c>
       <c r="C25" t="n">
-        <v>1376.350115796848</v>
+        <v>0.006041374974302016</v>
       </c>
     </row>
     <row r="26">
@@ -9204,7 +9204,7 @@
         <v>1946</v>
       </c>
       <c r="C26" t="n">
-        <v>137.6350115796853</v>
+        <v>0.0006041374974302017</v>
       </c>
     </row>
     <row r="27">
@@ -9215,7 +9215,7 @@
         <v>1947</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>6.041374908818398e-05</v>
       </c>
     </row>
     <row r="28">
@@ -9226,7 +9226,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>669.1001049000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -9237,7 +9237,7 @@
         <v>1949</v>
       </c>
       <c r="C29" t="n">
-        <v>558.8106598479671</v>
+        <v>539.6400459000012</v>
       </c>
     </row>
     <row r="30">
@@ -9248,7 +9248,7 @@
         <v>1950</v>
       </c>
       <c r="C30" t="n">
-        <v>55.88106598479754</v>
+        <v>1064.123964731373</v>
       </c>
     </row>
     <row r="31">
@@ -9259,7 +9259,7 @@
         <v>1951</v>
       </c>
       <c r="C31" t="n">
-        <v>5.588106598480408</v>
+        <v>106.4123964731381</v>
       </c>
     </row>
     <row r="32">
@@ -9270,7 +9270,7 @@
         <v>1952</v>
       </c>
       <c r="C32" t="n">
-        <v>0.5588106598472223</v>
+        <v>10.64123964731316</v>
       </c>
     </row>
     <row r="33">
@@ -9281,7 +9281,7 @@
         <v>1953</v>
       </c>
       <c r="C33" t="n">
-        <v>0.05588106598406739</v>
+        <v>1.064123964731152</v>
       </c>
     </row>
     <row r="34">
@@ -9292,7 +9292,7 @@
         <v>1954</v>
       </c>
       <c r="C34" t="n">
-        <v>0.005588106598406739</v>
+        <v>0.1064123964722967</v>
       </c>
     </row>
     <row r="35">
@@ -9303,7 +9303,7 @@
         <v>1955</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0005588106600043829</v>
+        <v>0.0106412396478845</v>
       </c>
     </row>
     <row r="36">
@@ -9314,7 +9314,7 @@
         <v>1956</v>
       </c>
       <c r="C36" t="n">
-        <v>5.588106632785639e-05</v>
+        <v>0.001064123965443287</v>
       </c>
     </row>
     <row r="37">
@@ -9325,7 +9325,7 @@
         <v>1957</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>0.0001064123960532015</v>
       </c>
     </row>
     <row r="38">
@@ -9336,7 +9336,7 @@
         <v>1958</v>
       </c>
       <c r="C38" t="n">
-        <v>1230.809611688105</v>
+        <v>1.064124026015634e-05</v>
       </c>
     </row>
     <row r="39">
@@ -9347,7 +9347,7 @@
         <v>1959</v>
       </c>
       <c r="C39" t="n">
-        <v>123.0809611688113</v>
+        <v>1.064123534888495e-06</v>
       </c>
     </row>
     <row r="40">
@@ -9358,7 +9358,7 @@
         <v>1960</v>
       </c>
       <c r="C40" t="n">
-        <v>12.30809611688146</v>
+        <v>1.064125171978958e-07</v>
       </c>
     </row>
     <row r="41">
@@ -9369,7 +9369,7 @@
         <v>1961</v>
       </c>
       <c r="C41" t="n">
-        <v>1.230809611687983</v>
+        <v>1.064108801074326e-08</v>
       </c>
     </row>
     <row r="42">
@@ -9380,7 +9380,7 @@
         <v>1962</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1230809611683071</v>
+        <v>1.064108801074326e-09</v>
       </c>
     </row>
     <row r="43">
@@ -9391,7 +9391,7 @@
         <v>1963</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01230809611715813</v>
+        <v>1.064108801074326e-10</v>
       </c>
     </row>
     <row r="44">
@@ -9413,7 +9413,7 @@
         <v>1965</v>
       </c>
       <c r="C45" t="n">
-        <v>1547.495573909612</v>
+        <v>1547.494343100009</v>
       </c>
     </row>
     <row r="46">
@@ -9424,7 +9424,7 @@
         <v>1966</v>
       </c>
       <c r="C46" t="n">
-        <v>154.7495573909615</v>
+        <v>154.7494343100018</v>
       </c>
     </row>
     <row r="47">
@@ -9435,7 +9435,7 @@
         <v>1967</v>
       </c>
       <c r="C47" t="n">
-        <v>15.47495573909582</v>
+        <v>15.47494343099952</v>
       </c>
     </row>
     <row r="48">
@@ -9446,7 +9446,7 @@
         <v>1968</v>
       </c>
       <c r="C48" t="n">
-        <v>1.547495573910237</v>
+        <v>1.547494343099788</v>
       </c>
     </row>
     <row r="49">
@@ -9457,7 +9457,7 @@
         <v>1969</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1547495573911874</v>
+        <v>0.1547494343098151</v>
       </c>
     </row>
     <row r="50">
@@ -9468,7 +9468,7 @@
         <v>1970</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01547495573977358</v>
+        <v>0.01547494343049038</v>
       </c>
     </row>
     <row r="51">
@@ -9479,7 +9479,7 @@
         <v>1971</v>
       </c>
       <c r="C51" t="n">
-        <v>0.001547495573322521</v>
+        <v>0.001547494342230493</v>
       </c>
     </row>
     <row r="52">
@@ -9490,7 +9490,7 @@
         <v>1972</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0001547495579870883</v>
+        <v>0.0001547494335682131</v>
       </c>
     </row>
     <row r="53">
@@ -9501,7 +9501,7 @@
         <v>1973</v>
       </c>
       <c r="C53" t="n">
-        <v>1.547495612612693e-05</v>
+        <v>1.547494302940322e-05</v>
       </c>
     </row>
     <row r="54">
@@ -9512,7 +9512,7 @@
         <v>1974</v>
       </c>
       <c r="C54" t="n">
-        <v>1.547495776321739e-06</v>
+        <v>1.547494139231276e-06</v>
       </c>
     </row>
     <row r="55">
@@ -9655,7 +9655,7 @@
         <v>1987</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>3.099599962297362e-06</v>
       </c>
     </row>
     <row r="68">
@@ -9666,7 +9666,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>422.7835868999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -9721,7 +9721,7 @@
         <v>1993</v>
       </c>
       <c r="C73" t="n">
-        <v>3799.424377479601</v>
+        <v>3888.610200899999</v>
       </c>
     </row>
     <row r="74">
@@ -9743,7 +9743,7 @@
         <v>1995</v>
       </c>
       <c r="C75" t="n">
-        <v>830.1518038479584</v>
+        <v>1635.117403089961</v>
       </c>
     </row>
     <row r="76">
@@ -9754,7 +9754,7 @@
         <v>1996</v>
       </c>
       <c r="C76" t="n">
-        <v>83.01518038479536</v>
+        <v>163.5117403089966</v>
       </c>
     </row>
     <row r="77">
@@ -9765,7 +9765,7 @@
         <v>1997</v>
       </c>
       <c r="C77" t="n">
-        <v>8.301518038480026</v>
+        <v>16.35117403089917</v>
       </c>
     </row>
     <row r="78">
@@ -9776,7 +9776,7 @@
         <v>1998</v>
       </c>
       <c r="C78" t="n">
-        <v>0.8301518038471841</v>
+        <v>1.635117403090408</v>
       </c>
     </row>
     <row r="79">
@@ -9787,7 +9787,7 @@
         <v>1999</v>
       </c>
       <c r="C79" t="n">
-        <v>0.08301518038406357</v>
+        <v>0.1635117403096956</v>
       </c>
     </row>
     <row r="80">
@@ -9798,7 +9798,7 @@
         <v>2000</v>
       </c>
       <c r="C80" t="n">
-        <v>0.008301518038570066</v>
+        <v>0.01635117403129698</v>
       </c>
     </row>
     <row r="81">
@@ -9820,7 +9820,7 @@
         <v>2002</v>
       </c>
       <c r="C82" t="n">
-        <v>373.9102032518031</v>
+        <v>373.911008217402</v>
       </c>
     </row>
     <row r="83">
@@ -9831,7 +9831,7 @@
         <v>2003</v>
       </c>
       <c r="C83" t="n">
-        <v>37.39102032517949</v>
+        <v>37.39110082173939</v>
       </c>
     </row>
     <row r="84">
@@ -9842,7 +9842,7 @@
         <v>2004</v>
       </c>
       <c r="C84" t="n">
-        <v>3.739102032517621</v>
+        <v>3.739110082173283</v>
       </c>
     </row>
     <row r="85">
@@ -9853,7 +9853,7 @@
         <v>2005</v>
       </c>
       <c r="C85" t="n">
-        <v>0.3739102032517622</v>
+        <v>0.3739110082173284</v>
       </c>
     </row>
     <row r="86">
@@ -9864,7 +9864,7 @@
         <v>2006</v>
       </c>
       <c r="C86" t="n">
-        <v>0.03739102032468509</v>
+        <v>0.03739110082206026</v>
       </c>
     </row>
     <row r="87">
@@ -9875,7 +9875,7 @@
         <v>2007</v>
       </c>
       <c r="C87" t="n">
-        <v>0.003739102031977381</v>
+        <v>0.003739110081551189</v>
       </c>
     </row>
     <row r="88">
@@ -9886,7 +9886,7 @@
         <v>2008</v>
       </c>
       <c r="C88" t="n">
-        <v>0.0003739102028703201</v>
+        <v>0.000373911008318828</v>
       </c>
     </row>
     <row r="89">
@@ -9908,7 +9908,7 @@
         <v>2010</v>
       </c>
       <c r="C90" t="n">
-        <v>435.8413417910195</v>
+        <v>435.8413417910997</v>
       </c>
     </row>
     <row r="91">
@@ -9919,7 +9919,7 @@
         <v>2011</v>
       </c>
       <c r="C91" t="n">
-        <v>43.58413417910179</v>
+        <v>43.58413417910997</v>
       </c>
     </row>
     <row r="92">
@@ -9930,7 +9930,7 @@
         <v>2012</v>
       </c>
       <c r="C92" t="n">
-        <v>4.358413417910015</v>
+        <v>4.358413417911652</v>
       </c>
     </row>
     <row r="93">
@@ -10021,7 +10021,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>6671.407475</v>
+        <v>1925.197475</v>
       </c>
     </row>
     <row r="5">
@@ -10109,7 +10109,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>2226.237236999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -10120,7 +10120,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>3663.060124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -10285,7 +10285,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>337.5554389999998</v>
       </c>
     </row>
     <row r="29">
@@ -10725,7 +10725,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>2554.450459</v>
       </c>
     </row>
     <row r="69">
@@ -11080,7 +11080,7 @@
         <v>1924</v>
       </c>
       <c r="C4" t="n">
-        <v>3937.8999999</v>
+        <v>1925.197475</v>
       </c>
     </row>
     <row r="5">
@@ -11168,7 +11168,7 @@
         <v>1932</v>
       </c>
       <c r="C12" t="n">
-        <v>2226.237236999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -11179,7 +11179,7 @@
         <v>1933</v>
       </c>
       <c r="C13" t="n">
-        <v>3663.060124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -11344,7 +11344,7 @@
         <v>1948</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>337.5554389999998</v>
       </c>
     </row>
     <row r="29">
@@ -11784,7 +11784,7 @@
         <v>1988</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>2554.450459</v>
       </c>
     </row>
     <row r="69">

</xml_diff>